<commit_message>
init biomass for NSH
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="3D_init_changer" sheetId="1" r:id="rId1"/>
@@ -25,95 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="24">
   <si>
     <t xml:space="preserve"> Loligo_Squid_N1 =</t>
   </si>
   <si>
-    <t xml:space="preserve">  0, 0, 0, 0, 0,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> _</t>
   </si>
   <si>
-    <t xml:space="preserve">  0.016, 0.016,  _,  _, 0.016,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.01475105,  _,  _,  _, 0.01475105,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0228227984,  _,  _,  _, 0.0228227984,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0110907496, 0.0110907496, 0.0110907496,  _, 0.0110907496,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0093838456,  _,  _,  _, 0.0093838456,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.006953258, 0.006953258,  _,  _, 0.006953258,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.007153652, 0.007153652,  _,  _, 0.007153652,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.021372518,  _,  _,  _, 0.021372518,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0079767192, 0.0079767192,  _,  _, 0.0079767192,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0079509948, 0.0079509948,  _,  _, 0.0079509948,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0031963188, 0.0031963188,  _,  _, 0.0031963188,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0006578772, 0.0006578772, 0.0006578772,  _, 0.0006578772,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0046369632, 0.0046369632,  _,  _, 0.0046369632,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.006613456,  _,  _,  _, 0.006613456,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0023099956, 0.0023099956, 0.0023099956,  _, 0.0023099956,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.002205892, 0.002205892,  _,  _, 0.002205892,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0004289828, 0.0004289828, 0.0004289828,  _, 0.0004289828,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0058717228, 0.0058717228,  _,  _, 0.0058717228,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.031125718, 0.031125718,  _,  _, 0.031125718,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.000236848, 0.000236848, 0.000236848,  _, 0.000236848,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0002237908, 0.0002237908, 0.0002237908,  _, 0.0002237908,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.000477548, 0.000477548, 0.000477548,  _, 0.000477548,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0003706108, 0.0003706108,  _,  _, 0.0003706108,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.002, 0.002, 0.002, 0.002, 0.002,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.004, 0.004, 0.004, 0.004, 0.004,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.008, 0.008, 0.008, 0.008, 0.008 ;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Scallop_N =</t>
   </si>
   <si>
@@ -130,6 +49,54 @@
   </si>
   <si>
     <t xml:space="preserve"> Filter_Other_N =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    _,   _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    _,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0152867011391446, 0.0152867011391446,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0105544135686993, 0.0105544135686993,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00285317221939058, 0.00285317221939058, 0.00285317221939058,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0072408337285406, 0.0072408337285406,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.032490819899342,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00339632574160188, 0.00339632574160188, 0.00339632574160188,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00970014391404955, 0.00970014391404955,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00919632787901202, 0.00919632787901202,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00265715716831268, 0.00265715716831268, 0.00265715716831268,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00230193597522717, 0.00230193597522717, 0.00230193597522717,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00284439848042167, 0.00284439848042167, 0.00284439848042167,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00664195018989087, 0.00664195018989087,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   _,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   _,  _,  _,  _,  _ ; ;</t>
   </si>
 </sst>
 </file>
@@ -145,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,8 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,33 +434,33 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="B2">
-        <v>3.2000000000000001E-2</v>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
         <f>IF(ISNUMBER(A2),A2*$G$1, A2)</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="H2">
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H2" t="str">
         <f t="shared" ref="H2:K17" si="0">IF(ISNUMBER(B2),B2*$G$1, B2)</f>
-        <v>1.6E-2</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="0"/>
@@ -495,37 +470,37 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K2">
-        <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M29" si="1">"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
-        <v xml:space="preserve">  0.016, 0.016,  _,  _, 0.016,</v>
+        <v xml:space="preserve">    _,   _,  _,  _,   _,</v>
       </c>
       <c r="T2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2.95021E-2</v>
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2.95021E-2</v>
-      </c>
-      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
         <f t="shared" ref="G3:G30" si="2">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
-        <v>1.475105E-2</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -539,37 +514,37 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>1.475105E-2</v>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.01475105,  _,  _,  _, 0.01475105,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4.56455968E-2</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4.56455968E-2</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
-        <v>2.28227984E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -583,81 +558,81 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>2.28227984E-2</v>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0228227984,  _,  _,  _, 0.0228227984,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2.21814992E-2</v>
-      </c>
-      <c r="B5">
-        <v>2.21814992E-2</v>
-      </c>
-      <c r="C5">
-        <v>2.21814992E-2</v>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2.21814992E-2</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>1.10907496E-2</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>1.10907496E-2</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>1.10907496E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1.10907496E-2</v>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0110907496, 0.0110907496, 0.0110907496,  _, 0.0110907496,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.8767691199999999E-2</v>
+      <c r="A6" t="s">
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>1.8767691199999999E-2</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>9.3838455999999994E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -671,41 +646,41 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>9.3838455999999994E-3</v>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0093838456,  _,  _,  _, 0.0093838456,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1.3906516000000001E-2</v>
-      </c>
-      <c r="B7">
-        <v>1.3906516000000001E-2</v>
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1.3906516000000001E-2</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>6.9532580000000004E-3</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>6.9532580000000004E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -715,41 +690,41 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>6.9532580000000004E-3</v>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.006953258, 0.006953258,  _,  _, 0.006953258,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1.4307304E-2</v>
-      </c>
-      <c r="B8">
-        <v>1.4307304E-2</v>
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>1.4307304E-2</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>7.1536519999999999E-3</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>7.1536519999999999E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -759,37 +734,37 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>7.1536519999999999E-3</v>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.007153652, 0.007153652,  _,  _, 0.007153652,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4.2745036E-2</v>
+      <c r="A9" t="s">
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>4.2745036E-2</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>2.1372518E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -803,85 +778,85 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>2.1372518E-2</v>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.021372518,  _,  _,  _, 0.021372518,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>3.0573402278289169E-2</v>
+      </c>
+      <c r="B10">
+        <v>3.0573402278289169E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>1.5286701139144585E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1.5286701139144585E-2</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  0.0152867011391446, 0.0152867011391446,  _,  _,   _,</v>
+      </c>
+      <c r="T10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1.5953438399999999E-2</v>
-      </c>
-      <c r="B10">
-        <v>1.5953438399999999E-2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>1.5953438399999999E-2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>7.9767191999999994E-3</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>7.9767191999999994E-3</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>7.9767191999999994E-3</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0079767192, 0.0079767192,  _,  _, 0.0079767192,</v>
-      </c>
-      <c r="T10" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1.5901989599999999E-2</v>
-      </c>
-      <c r="B11">
-        <v>1.5901989599999999E-2</v>
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>1.5901989599999999E-2</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>7.9509947999999997E-3</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>7.9509947999999997E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -891,41 +866,41 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>7.9509947999999997E-3</v>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0079509948, 0.0079509948,  _,  _, 0.0079509948,</v>
+        <v xml:space="preserve">    _,   _,  _,  _,   _,</v>
       </c>
       <c r="T11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6.3926375999999998E-3</v>
+        <v>2.1108827137398572E-2</v>
       </c>
       <c r="B12">
-        <v>6.3926375999999998E-3</v>
+        <v>2.1108827137398572E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>6.3926375999999998E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>3.1963187999999999E-3</v>
+        <v>1.0554413568699286E-2</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>3.1963187999999999E-3</v>
+        <v>1.0554413568699286E-2</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -935,85 +910,85 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>3.1963187999999999E-3</v>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0031963188, 0.0031963188,  _,  _, 0.0031963188,</v>
+        <v xml:space="preserve">  0.0105544135686993, 0.0105544135686993,  _,  _,   _,</v>
       </c>
       <c r="T12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1.3157544000000001E-3</v>
+        <v>5.7063444387811567E-3</v>
       </c>
       <c r="B13">
-        <v>1.3157544000000001E-3</v>
+        <v>5.7063444387811567E-3</v>
       </c>
       <c r="C13">
-        <v>1.3157544000000001E-3</v>
+        <v>5.7063444387811567E-3</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>1.3157544000000001E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>6.5787720000000003E-4</v>
+        <v>2.8531722193905784E-3</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>6.5787720000000003E-4</v>
+        <v>2.8531722193905784E-3</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>6.5787720000000003E-4</v>
+        <v>2.8531722193905784E-3</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>6.5787720000000003E-4</v>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0006578772, 0.0006578772, 0.0006578772,  _, 0.0006578772,</v>
+        <v xml:space="preserve">  0.00285317221939058, 0.00285317221939058, 0.00285317221939058,  _,   _,</v>
       </c>
       <c r="T13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9.2739264000000002E-3</v>
+        <v>1.4481667457081206E-2</v>
       </c>
       <c r="B14">
-        <v>9.2739264000000002E-3</v>
+        <v>1.4481667457081206E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>9.2739264000000002E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>4.6369632000000001E-3</v>
+        <v>7.2408337285406032E-3</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>4.6369632000000001E-3</v>
+        <v>7.2408337285406032E-3</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -1023,37 +998,37 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>4.6369632000000001E-3</v>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0046369632, 0.0046369632,  _,  _, 0.0046369632,</v>
+        <v xml:space="preserve">  0.0072408337285406, 0.0072408337285406,  _,  _,   _,</v>
       </c>
       <c r="T14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1.3226912E-2</v>
+        <v>6.4981639798683988E-2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>1.3226912E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>6.6134560000000002E-3</v>
+        <v>3.2490819899341994E-2</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1067,85 +1042,85 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>6.6134560000000002E-3</v>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.006613456,  _,  _,  _, 0.006613456,</v>
+        <v xml:space="preserve">  0.032490819899342,  _,  _,  _,   _,</v>
       </c>
       <c r="T15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4.6199911999999996E-3</v>
-      </c>
-      <c r="B16">
-        <v>4.6199911999999996E-3</v>
-      </c>
-      <c r="C16">
-        <v>4.6199911999999996E-3</v>
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>4.6199911999999996E-3</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="2"/>
-        <v>2.3099955999999998E-3</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>2.3099955999999998E-3</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>2.3099955999999998E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>2.3099955999999998E-3</v>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0023099956, 0.0023099956, 0.0023099956,  _, 0.0023099956,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4.4117840000000002E-3</v>
-      </c>
-      <c r="B17">
-        <v>4.4117840000000002E-3</v>
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>4.4117840000000002E-3</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
-        <v>2.2058920000000001E-3</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>2.2058920000000001E-3</v>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -1155,85 +1130,85 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>2.2058920000000001E-3</v>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.002205892, 0.002205892,  _,  _, 0.002205892,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T17" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>8.5796560000000002E-4</v>
+        <v>6.7926514832037542E-3</v>
       </c>
       <c r="B18">
-        <v>8.5796560000000002E-4</v>
+        <v>6.7926514832037542E-3</v>
       </c>
       <c r="C18">
-        <v>8.5796560000000002E-4</v>
+        <v>6.7926514832037542E-3</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>8.5796560000000002E-4</v>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>4.2898280000000001E-4</v>
+        <v>3.3963257416018771E-3</v>
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H31" si="3">IF(ISNUMBER(B18),B18*$G$1, B18)</f>
-        <v>4.2898280000000001E-4</v>
+        <v>3.3963257416018771E-3</v>
       </c>
       <c r="I18">
         <f t="shared" ref="I18:I31" si="4">IF(ISNUMBER(C18),C18*$G$1, C18)</f>
-        <v>4.2898280000000001E-4</v>
+        <v>3.3963257416018771E-3</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ref="J18:J31" si="5">IF(ISNUMBER(D18),D18*$G$1, D18)</f>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K18">
+      <c r="K18" t="str">
         <f t="shared" ref="K18:K31" si="6">IF(ISNUMBER(E18),E18*$G$1, E18)</f>
-        <v>4.2898280000000001E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0004289828, 0.0004289828, 0.0004289828,  _, 0.0004289828,</v>
+        <v xml:space="preserve">  0.00339632574160188, 0.00339632574160188, 0.00339632574160188,  _,   _,</v>
       </c>
       <c r="T18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1.1743445599999999E-2</v>
-      </c>
-      <c r="B19">
-        <v>1.1743445599999999E-2</v>
+        <v>1.9400287828099102E-2</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.9400287828099102E-2</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>1.1743445599999999E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>5.8717227999999996E-3</v>
+        <v>9.7001439140495509E-3</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>5.8717227999999996E-3</v>
+        <v>9.7001439140495509E-3</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="4"/>
@@ -1243,41 +1218,41 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K19">
+      <c r="K19" t="str">
         <f t="shared" si="6"/>
-        <v>5.8717227999999996E-3</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0058717228, 0.0058717228,  _,  _, 0.0058717228,</v>
+        <v xml:space="preserve">  0.00970014391404955, 0.00970014391404955,  _,  _,   _,</v>
       </c>
       <c r="T19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6.2251436E-2</v>
-      </c>
-      <c r="B20">
-        <v>6.2251436E-2</v>
+        <v>1.8392655758024037E-2</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.8392655758024037E-2</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>6.2251436E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>3.1125718E-2</v>
+        <v>9.1963278790120184E-3</v>
       </c>
       <c r="H20">
         <f t="shared" si="3"/>
-        <v>3.1125718E-2</v>
+        <v>9.1963278790120184E-3</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="4"/>
@@ -1287,173 +1262,173 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K20">
+      <c r="K20" t="str">
         <f t="shared" si="6"/>
-        <v>3.1125718E-2</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.031125718, 0.031125718,  _,  _, 0.031125718,</v>
+        <v xml:space="preserve">  0.00919632787901202, 0.00919632787901202,  _,  _,   _,</v>
       </c>
       <c r="T20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4.7369600000000001E-4</v>
+        <v>5.3143143366253523E-3</v>
       </c>
       <c r="B21">
-        <v>4.7369600000000001E-4</v>
+        <v>5.3143143366253523E-3</v>
       </c>
       <c r="C21">
-        <v>4.7369600000000001E-4</v>
+        <v>5.3143143366253523E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>4.7369600000000001E-4</v>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>2.3684800000000001E-4</v>
+        <v>2.6571571683126761E-3</v>
       </c>
       <c r="H21">
         <f t="shared" si="3"/>
-        <v>2.3684800000000001E-4</v>
+        <v>2.6571571683126761E-3</v>
       </c>
       <c r="I21">
         <f t="shared" si="4"/>
-        <v>2.3684800000000001E-4</v>
+        <v>2.6571571683126761E-3</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K21">
+      <c r="K21" t="str">
         <f t="shared" si="6"/>
-        <v>2.3684800000000001E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.000236848, 0.000236848, 0.000236848,  _, 0.000236848,</v>
+        <v xml:space="preserve">  0.00265715716831268, 0.00265715716831268, 0.00265715716831268,  _,   _,</v>
       </c>
       <c r="T21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4.475816E-4</v>
+        <v>4.6038719504543461E-3</v>
       </c>
       <c r="B22">
-        <v>4.475816E-4</v>
+        <v>4.6038719504543461E-3</v>
       </c>
       <c r="C22">
-        <v>4.475816E-4</v>
+        <v>4.6038719504543461E-3</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22">
-        <v>4.475816E-4</v>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>2.237908E-4</v>
+        <v>2.3019359752271731E-3</v>
       </c>
       <c r="H22">
         <f t="shared" si="3"/>
-        <v>2.237908E-4</v>
+        <v>2.3019359752271731E-3</v>
       </c>
       <c r="I22">
         <f t="shared" si="4"/>
-        <v>2.237908E-4</v>
+        <v>2.3019359752271731E-3</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K22">
+      <c r="K22" t="str">
         <f t="shared" si="6"/>
-        <v>2.237908E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0002237908, 0.0002237908, 0.0002237908,  _, 0.0002237908,</v>
+        <v xml:space="preserve">  0.00230193597522717, 0.00230193597522717, 0.00230193597522717,  _,   _,</v>
       </c>
       <c r="T22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9.55096E-4</v>
+        <v>5.6887969608433314E-3</v>
       </c>
       <c r="B23">
-        <v>9.55096E-4</v>
+        <v>5.6887969608433314E-3</v>
       </c>
       <c r="C23">
-        <v>9.55096E-4</v>
+        <v>5.6887969608433314E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <v>9.55096E-4</v>
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>4.77548E-4</v>
+        <v>2.8443984804216657E-3</v>
       </c>
       <c r="H23">
         <f t="shared" si="3"/>
-        <v>4.77548E-4</v>
+        <v>2.8443984804216657E-3</v>
       </c>
       <c r="I23">
         <f t="shared" si="4"/>
-        <v>4.77548E-4</v>
+        <v>2.8443984804216657E-3</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K23">
+      <c r="K23" t="str">
         <f t="shared" si="6"/>
-        <v>4.77548E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.000477548, 0.000477548, 0.000477548,  _, 0.000477548,</v>
+        <v xml:space="preserve">  0.00284439848042167, 0.00284439848042167, 0.00284439848042167,  _,   _,</v>
       </c>
       <c r="T23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>7.4122160000000001E-4</v>
-      </c>
-      <c r="B24">
-        <v>7.4122160000000001E-4</v>
+        <v>1.3283900379781735E-2</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.3283900379781735E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <v>7.4122160000000001E-4</v>
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>3.7061080000000001E-4</v>
+        <v>6.6419501898908676E-3</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
-        <v>3.7061080000000001E-4</v>
+        <v>6.6419501898908676E-3</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="4"/>
@@ -1463,129 +1438,129 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K24">
+      <c r="K24" t="str">
         <f t="shared" si="6"/>
-        <v>3.7061080000000001E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0003706108, 0.0003706108,  _,  _, 0.0003706108,</v>
+        <v xml:space="preserve">  0.00664195018989087, 0.00664195018989087,  _,  _,   _,</v>
       </c>
       <c r="T24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H25" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I25">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I25" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J25">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K25">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K25" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T25" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H26">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="H26" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I26">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I26" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J26">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J26" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K26">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K26" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
       </c>
       <c r="T26" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>7.4122160000000001E-4</v>
-      </c>
-      <c r="B27">
-        <v>7.4122160000000001E-4</v>
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27">
-        <v>7.4122160000000001E-4</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="2"/>
-        <v>3.7061080000000001E-4</v>
-      </c>
-      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H27" t="str">
         <f t="shared" si="3"/>
-        <v>3.7061080000000001E-4</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="4"/>
@@ -1595,192 +1570,192 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K27">
+      <c r="K27" t="str">
         <f t="shared" si="6"/>
-        <v>3.7061080000000001E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0003706108, 0.0003706108,  _,  _, 0.0003706108,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T27" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>9.55096E-4</v>
-      </c>
-      <c r="B28">
-        <v>9.55096E-4</v>
-      </c>
-      <c r="C28">
-        <v>9.55096E-4</v>
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>9.55096E-4</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="2"/>
-        <v>4.77548E-4</v>
-      </c>
-      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="H28" t="str">
         <f t="shared" si="3"/>
-        <v>4.77548E-4</v>
-      </c>
-      <c r="I28">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I28" t="str">
         <f t="shared" si="4"/>
-        <v>4.77548E-4</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> _</v>
       </c>
-      <c r="K28">
+      <c r="K28" t="str">
         <f t="shared" si="6"/>
-        <v>4.77548E-4</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.000477548, 0.000477548, 0.000477548,  _, 0.000477548,</v>
+        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
       </c>
       <c r="T28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="B29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="2"/>
-        <v>2E-3</v>
-      </c>
-      <c r="H29">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _</v>
+      </c>
+      <c r="H29" t="str">
         <f t="shared" si="3"/>
-        <v>2E-3</v>
-      </c>
-      <c r="I29">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I29" t="str">
         <f t="shared" si="4"/>
-        <v>2E-3</v>
-      </c>
-      <c r="J29">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J29" t="str">
         <f t="shared" si="5"/>
-        <v>2E-3</v>
-      </c>
-      <c r="K29">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K29" t="str">
         <f t="shared" si="6"/>
-        <v>2E-3</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.002, 0.002, 0.002, 0.002, 0.002,</v>
+        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
       </c>
       <c r="T29" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="B30">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C30">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D30">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E30">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="2"/>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H30">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="H30" t="str">
         <f t="shared" si="3"/>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I30">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I30" t="str">
         <f t="shared" si="4"/>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="J30">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="5"/>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="K30">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K30" t="str">
         <f t="shared" si="6"/>
-        <v>4.0000000000000001E-3</v>
+        <v xml:space="preserve">  _</v>
       </c>
       <c r="M30" t="str">
         <f>"  "&amp;G30&amp;", "&amp;H30&amp;", "&amp;I30&amp;", "&amp;J30&amp;", "&amp;K30&amp;","</f>
-        <v xml:space="preserve">  0.004, 0.004, 0.004, 0.004, 0.004,</v>
+        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
       </c>
       <c r="T30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1.6E-2</v>
-      </c>
-      <c r="B31">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C31">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D31">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E31">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G31">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" t="str">
         <f>IF(ISNUMBER(A31),A31*$G$1, A31)</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H31">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="H31" t="str">
         <f t="shared" si="3"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I31">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I31" t="str">
         <f t="shared" si="4"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J31">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="J31" t="str">
         <f t="shared" si="5"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K31">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="K31" t="str">
         <f t="shared" si="6"/>
-        <v>8.0000000000000002E-3</v>
+        <v xml:space="preserve"> _ ;</v>
       </c>
       <c r="M31" t="str">
         <f>"  "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;" ;"</f>
-        <v xml:space="preserve">  0.008, 0.008, 0.008, 0.008, 0.008 ;</v>
+        <v xml:space="preserve">   _,  _,  _,  _,  _ ; ;</v>
       </c>
       <c r="T31" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -1800,12 +1775,12 @@
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0.71199999999999997</v>
@@ -1838,7 +1813,7 @@
         <v>0.56200000000000006</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1873,7 +1848,7 @@
         <v>0.56200000000000006</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1890,24 +1865,24 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -2137,7 +2112,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to invert biomass init vals, calc and sources updated in xls
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -12,8 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="3D_init_changer" sheetId="1" r:id="rId1"/>
-    <sheet name="2D_init_changer" sheetId="2" r:id="rId2"/>
+    <sheet name="2D calc" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="3D_init_changer" sheetId="1" r:id="rId3"/>
+    <sheet name="2D_init_changer" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="48">
   <si>
     <t xml:space="preserve"> Loligo_Squid_N1 =</t>
   </si>
@@ -97,13 +99,85 @@
   </si>
   <si>
     <t xml:space="preserve">   _,  _,  _,  _,  _ ; ;</t>
+  </si>
+  <si>
+    <t>total NEUS biomass in mg</t>
+  </si>
+  <si>
+    <t>Box area (m2)</t>
+  </si>
+  <si>
+    <t>(paste scalar here)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 67.1800620400568, 67.169624003467, 67.2106814919619, 67.1100631326957, 67.2183511878286, 67.2072937091949, 67.2188746729358, 67.1256052351668, 0, 0, 0, 0, 67.2066000827306, 0, 67.2090784058426, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t>CLA</t>
+  </si>
+  <si>
+    <t>SPP</t>
+  </si>
+  <si>
+    <t>totalBiomass(mg)</t>
+  </si>
+  <si>
+    <t>Init_entry</t>
+  </si>
+  <si>
+    <t>NOAA TM142</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>VALUES SAVED HERE RM 20180823</t>
+  </si>
+  <si>
+    <t>XXX_N =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0, 286.941609468405, 0, 0, 286.924976095042, 287.06406178004, 287.161741675816, 286.982344649134, 287.115928093719, 0, 0, 286.779016476727, 287.161104132294, 0, 287.192135890684, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t>QHG</t>
+  </si>
+  <si>
+    <t>NOAA TM148</t>
+  </si>
+  <si>
+    <t>SEE 'spring_invert_PA_scaled_Atl_boxes.xlsx' for biomass scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0.0941, 0.2295, 0.1068, 0.0282, 0.0849, 0.1489, 0.0794, 0.0494, 0, 0, 0, 0, 0.1085, 0, 0.0703, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t>Scalar, also used for XXX_cover</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.088379386, 0, 0, 0, 0, 0.088379386, 0, 0.088379386, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>RCB</t>
+  </si>
+  <si>
+    <t>CRD 06-25 p369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 3.47237897680724E-05, 0.0166036077, 0.1179608232, 0.0042714077, 0.0006875969, 0.001671102, 0.0035984742, 0.1650576391, 0.0058367059, 0.0040807738, 0.0928870725, 0.000132936, 0.0479163159, 0.0128213926, 0.0156118159, 0.0055771748, NA, 0.0147174501, 0.0395492518, 0.0490960392, 0.176187393, 0.2108153867, 0.0069150329, 4.82114043340968E-19, 0.0013114908, 0.002527667, 0.0004194573, 0.0024787444, 0.0012325248, NA ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +185,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC5C8C6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +227,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1D1F21"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -134,14 +242,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,9 +565,997 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>12647072876</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12286957937</v>
+      </c>
+      <c r="C2" s="3">
+        <v>29971254486</v>
+      </c>
+      <c r="D2" s="3">
+        <v>13938887160</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3686010853</v>
+      </c>
+      <c r="F2" s="3">
+        <v>11079367895</v>
+      </c>
+      <c r="G2" s="3">
+        <v>19434502995</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10361542520</v>
+      </c>
+      <c r="I2" s="3">
+        <v>6455559422</v>
+      </c>
+      <c r="J2" s="3">
+        <v>17316802511</v>
+      </c>
+      <c r="K2" s="3">
+        <v>11225017827</v>
+      </c>
+      <c r="L2" s="3">
+        <v>15989283041</v>
+      </c>
+      <c r="M2" s="3">
+        <v>4282287423</v>
+      </c>
+      <c r="N2" s="3">
+        <v>14161620805</v>
+      </c>
+      <c r="O2" s="3">
+        <v>12608709589</v>
+      </c>
+      <c r="P2" s="3">
+        <v>9175347755</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>11324453301</v>
+      </c>
+      <c r="R2" s="3">
+        <v>5030841128</v>
+      </c>
+      <c r="S2" s="3">
+        <v>4831356901</v>
+      </c>
+      <c r="T2" s="3">
+        <v>17683470543</v>
+      </c>
+      <c r="U2" s="3">
+        <v>9957085306</v>
+      </c>
+      <c r="V2" s="3">
+        <v>6033778736</v>
+      </c>
+      <c r="W2" s="3">
+        <v>17242902545</v>
+      </c>
+      <c r="X2" s="3">
+        <v>173026053</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>294595432</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>35556339824</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>17529276725</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>26033456848</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>40232596619</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>27427742420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="C4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="F4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="G4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="H4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="I4">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="K4">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="B5">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="G5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="H5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="I5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="J5">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="B6">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>3.4723789768072398E-5</v>
+      </c>
+      <c r="C11">
+        <v>1.6603607699999998E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.1179608232</v>
+      </c>
+      <c r="E11">
+        <v>4.2714077000000003E-3</v>
+      </c>
+      <c r="F11">
+        <v>6.8759690000000004E-4</v>
+      </c>
+      <c r="G11">
+        <v>1.671102E-3</v>
+      </c>
+      <c r="H11">
+        <v>3.5984742E-3</v>
+      </c>
+      <c r="I11">
+        <v>0.16505763909999999</v>
+      </c>
+      <c r="J11">
+        <v>5.8367059000000001E-3</v>
+      </c>
+      <c r="K11">
+        <v>4.0807737999999996E-3</v>
+      </c>
+      <c r="L11">
+        <v>9.2887072500000001E-2</v>
+      </c>
+      <c r="M11">
+        <v>1.32936E-4</v>
+      </c>
+      <c r="N11">
+        <v>4.7916315899999999E-2</v>
+      </c>
+      <c r="O11">
+        <v>1.28213926E-2</v>
+      </c>
+      <c r="P11">
+        <v>1.5611815899999999E-2</v>
+      </c>
+      <c r="Q11">
+        <v>5.5771748000000001E-3</v>
+      </c>
+      <c r="R11" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11">
+        <v>1.47174501E-2</v>
+      </c>
+      <c r="T11">
+        <v>3.9549251799999997E-2</v>
+      </c>
+      <c r="U11">
+        <v>4.9096039199999997E-2</v>
+      </c>
+      <c r="V11">
+        <v>0.176187393</v>
+      </c>
+      <c r="W11">
+        <v>0.2108153867</v>
+      </c>
+      <c r="X11">
+        <v>6.9150328999999996E-3</v>
+      </c>
+      <c r="Y11">
+        <v>4.8211404334096802E-19</v>
+      </c>
+      <c r="Z11">
+        <v>1.3114908000000001E-3</v>
+      </c>
+      <c r="AA11">
+        <v>2.5276669999999999E-3</v>
+      </c>
+      <c r="AB11">
+        <v>4.1945730000000003E-4</v>
+      </c>
+      <c r="AC11">
+        <v>2.4787443999999999E-3</v>
+      </c>
+      <c r="AD11">
+        <v>1.2325248000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>63000000000000</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="15" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <f>$A$13*A11/20/5.7/A2</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" ref="B15:AD15" si="0">$A$13*B11/20/5.7/B2</f>
+        <v>1.5617749214214083E-3</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30614927859492075</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6767633047506045</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.64039821794278029</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>3.429688084442075E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7518773033696775E-2</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19192417297992889</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>14.1298465013429</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18626695057124343</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20090520150414479</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2104209680850873</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7155464900457561E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8698473626555978</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.56195333763762723</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94030032445921519</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27216527225356729</v>
+      </c>
+      <c r="R15" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6834458421315674</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2359658368686464</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7248959740064214</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="0"/>
+        <v>16.136938632383174</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7565909924024945</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="0"/>
+        <v>22.086070182737163</v>
+      </c>
+      <c r="Y15" s="2">
+        <f t="shared" si="0"/>
+        <v>9.0439774709140483E-16</v>
+      </c>
+      <c r="Z15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0383741272765581E-2</v>
+      </c>
+      <c r="AA15" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9687749082708245E-2</v>
+      </c>
+      <c r="AB15" s="2">
+        <f t="shared" si="0"/>
+        <v>8.9041325304368198E-3</v>
+      </c>
+      <c r="AC15" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4047825561724712E-2</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4833692685516676E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <f>IF(ISNUMBER(A15),A15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.22950000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="E16">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>8.4900000000000003E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.1489</v>
+      </c>
+      <c r="H16">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="I16">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0.1085</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>7.0300000000000001E-2</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>"  "&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;G16&amp;", "&amp;H16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;", "&amp;P16&amp;", "&amp;Q16&amp;", "&amp;R16&amp;", "&amp;S16&amp;", "&amp;T16&amp;", "&amp;U16&amp;", "&amp;V16&amp;", "&amp;W16&amp;", "&amp;X16&amp;", "&amp;Y16&amp;", "&amp;Z16&amp;", "&amp;AA16&amp;", "&amp;AB16&amp;", "&amp;AC16&amp;", "&amp;AD16&amp;", "&amp;R16&amp;" ;"</f>
+        <v xml:space="preserve">  0, 0.0941, 0.2295, 0.1068, 0.0282, 0.0849, 0.1489, 0.0794, 0.0494, 0, 0, 0, 0, 0.1085, 0, 0.0703, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>3.4723789768072398E-5</v>
+      </c>
+      <c r="C22">
+        <v>1.6603607699999998E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.1179608232</v>
+      </c>
+      <c r="E22">
+        <v>4.2714077000000003E-3</v>
+      </c>
+      <c r="F22">
+        <v>6.8759690000000004E-4</v>
+      </c>
+      <c r="G22">
+        <v>1.671102E-3</v>
+      </c>
+      <c r="H22">
+        <v>3.5984742E-3</v>
+      </c>
+      <c r="I22">
+        <v>0.16505763909999999</v>
+      </c>
+      <c r="J22">
+        <v>5.8367059000000001E-3</v>
+      </c>
+      <c r="K22">
+        <v>4.0807737999999996E-3</v>
+      </c>
+      <c r="L22">
+        <v>9.2887072500000001E-2</v>
+      </c>
+      <c r="M22">
+        <v>1.32936E-4</v>
+      </c>
+      <c r="N22">
+        <v>4.7916315899999999E-2</v>
+      </c>
+      <c r="O22">
+        <v>1.28213926E-2</v>
+      </c>
+      <c r="P22">
+        <v>1.5611815899999999E-2</v>
+      </c>
+      <c r="Q22">
+        <v>5.5771748000000001E-3</v>
+      </c>
+      <c r="R22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S22">
+        <v>1.47174501E-2</v>
+      </c>
+      <c r="T22">
+        <v>3.9549251799999997E-2</v>
+      </c>
+      <c r="U22">
+        <v>4.9096039199999997E-2</v>
+      </c>
+      <c r="V22">
+        <v>0.176187393</v>
+      </c>
+      <c r="W22">
+        <v>0.2108153867</v>
+      </c>
+      <c r="X22">
+        <v>6.9150328999999996E-3</v>
+      </c>
+      <c r="Y22">
+        <v>4.8211404334096802E-19</v>
+      </c>
+      <c r="Z22">
+        <v>1.3114908000000001E-3</v>
+      </c>
+      <c r="AA22">
+        <v>2.5276669999999999E-3</v>
+      </c>
+      <c r="AB22">
+        <v>4.1945730000000003E-4</v>
+      </c>
+      <c r="AC22">
+        <v>2.4787443999999999E-3</v>
+      </c>
+      <c r="AD22">
+        <v>1.2325248000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>"  "&amp;A22&amp;", "&amp;B22&amp;", "&amp;C22&amp;", "&amp;D22&amp;", "&amp;E22&amp;", "&amp;F22&amp;", "&amp;G22&amp;", "&amp;H22&amp;", "&amp;I22&amp;", "&amp;J22&amp;", "&amp;K22&amp;", "&amp;L22&amp;", "&amp;M22&amp;", "&amp;N22&amp;", "&amp;O22&amp;", "&amp;P22&amp;", "&amp;Q22&amp;", "&amp;R22&amp;", "&amp;S22&amp;", "&amp;T22&amp;", "&amp;U22&amp;", "&amp;V22&amp;", "&amp;W22&amp;", "&amp;X22&amp;", "&amp;Y22&amp;", "&amp;Z22&amp;", "&amp;AA22&amp;", "&amp;AB22&amp;", "&amp;AC22&amp;", "&amp;AD22&amp;", "&amp;R22&amp;" ;"</f>
+        <v xml:space="preserve">  0, 3.47237897680724E-05, 0.0166036077, 0.1179608232, 0.0042714077, 0.0006875969, 0.001671102, 0.0035984742, 0.1650576391, 0.0058367059, 0.0040807738, 0.0928870725, 0.000132936, 0.0479163159, 0.0128213926, 0.0156118159, 0.0055771748, NA, 0.0147174501, 0.0395492518, 0.0490960392, 0.176187393, 0.2108153867, 0.0069150329, 4.82114043340968E-19, 0.0013114908, 0.002527667, 0.0004194573, 0.0024787444, 0.0012325248, NA ;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1000000000000000</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4000000000000000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2">
+        <v>63000000000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AF17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>9.06E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.159</v>
+      </c>
+      <c r="H3">
+        <v>8.48E-2</v>
+      </c>
+      <c r="I3">
+        <v>5.28E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.14169999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N3">
+        <v>0.1159</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>7.51E-2</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.16340131599999999</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.16340131599999999</v>
+      </c>
+      <c r="G4">
+        <v>0.16340131599999999</v>
+      </c>
+      <c r="H4">
+        <v>0.16340131599999999</v>
+      </c>
+      <c r="I4">
+        <v>8.8379386000000004E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.16340131599999999</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>8.8379386000000004E-2</v>
+      </c>
+      <c r="N4">
+        <v>8.8379386000000004E-2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>8.8379386000000004E-2</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>"  "&amp;A4&amp;", "&amp;B4&amp;", "&amp;C4&amp;", "&amp;D4&amp;", "&amp;E4&amp;", "&amp;F4&amp;", "&amp;G4&amp;", "&amp;H4&amp;", "&amp;I4&amp;", "&amp;J4&amp;", "&amp;K4&amp;", "&amp;L4&amp;", "&amp;M4&amp;", "&amp;N4&amp;", "&amp;O4&amp;", "&amp;P4&amp;", "&amp;Q4&amp;", "&amp;R4&amp;", "&amp;S4&amp;", "&amp;T4&amp;", "&amp;U4&amp;", "&amp;V4&amp;", "&amp;W4&amp;", "&amp;X4&amp;", "&amp;Y4&amp;", "&amp;Z4&amp;", "&amp;AA4&amp;", "&amp;AB4&amp;", "&amp;AC4&amp;", "&amp;AD4&amp;", "&amp;R4&amp;" ;"</f>
+        <v xml:space="preserve">  0, 0, 0.163401316, 0, 0, 0.163401316, 0.163401316, 0.163401316, 0.088379386, 0.163401316, 0, 0, 0.088379386, 0.088379386, 0, 0.088379386, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
@@ -1763,16 +2894,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AD19"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3">
+        <v>12647072876</v>
+      </c>
+      <c r="B1" s="3">
+        <v>12286957937</v>
+      </c>
+      <c r="C1" s="3">
+        <v>29971254486</v>
+      </c>
+      <c r="D1" s="3">
+        <v>13938887160</v>
+      </c>
+      <c r="E1" s="3">
+        <v>3686010853</v>
+      </c>
+      <c r="F1" s="3">
+        <v>11079367895</v>
+      </c>
+      <c r="G1" s="3">
+        <v>19434502995</v>
+      </c>
+      <c r="H1" s="3">
+        <v>10361542520</v>
+      </c>
+      <c r="I1" s="3">
+        <v>6455559422</v>
+      </c>
+      <c r="J1" s="3">
+        <v>17316802511</v>
+      </c>
+      <c r="K1" s="3">
+        <v>11225017827</v>
+      </c>
+      <c r="L1" s="3">
+        <v>15989283041</v>
+      </c>
+      <c r="M1" s="3">
+        <v>4282287423</v>
+      </c>
+      <c r="N1" s="3">
+        <v>14161620805</v>
+      </c>
+      <c r="O1" s="3">
+        <v>12608709589</v>
+      </c>
+      <c r="P1" s="3">
+        <v>9175347755</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>11324453301</v>
+      </c>
+      <c r="R1" s="3">
+        <v>5030841128</v>
+      </c>
+      <c r="S1" s="3">
+        <v>4831356901</v>
+      </c>
+      <c r="T1" s="3">
+        <v>17683470543</v>
+      </c>
+      <c r="U1" s="3">
+        <v>9957085306</v>
+      </c>
+      <c r="V1" s="3">
+        <v>6033778736</v>
+      </c>
+      <c r="W1" s="3">
+        <v>17242902545</v>
+      </c>
+      <c r="X1" s="3">
+        <v>173026053</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>294595432</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>35556339824</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>17529276725</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>26033456848</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>40232596619</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>27427742420</v>
+      </c>
+    </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
@@ -1980,6 +3203,9 @@
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changes to init vals for benthic and LTL
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2D calc" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
   <si>
     <t xml:space="preserve"> Loligo_Squid_N1 =</t>
   </si>
@@ -53,54 +53,6 @@
     <t xml:space="preserve"> Filter_Other_N =</t>
   </si>
   <si>
-    <t xml:space="preserve">    _,   _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    _,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0152867011391446, 0.0152867011391446,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0105544135686993, 0.0105544135686993,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00285317221939058, 0.00285317221939058, 0.00285317221939058,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0072408337285406, 0.0072408337285406,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.032490819899342,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00339632574160188, 0.00339632574160188, 0.00339632574160188,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00970014391404955, 0.00970014391404955,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00919632787901202, 0.00919632787901202,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00265715716831268, 0.00265715716831268, 0.00265715716831268,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00230193597522717, 0.00230193597522717, 0.00230193597522717,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00284439848042167, 0.00284439848042167, 0.00284439848042167,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00664195018989087, 0.00664195018989087,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   _,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   _,  _,  _,  _,  _ ; ;</t>
-  </si>
-  <si>
     <t>total NEUS biomass in mg</t>
   </si>
   <si>
@@ -171,6 +123,78 @@
   </si>
   <si>
     <t xml:space="preserve">  0, 3.47237897680724E-05, 0.0166036077, 0.1179608232, 0.0042714077, 0.0006875969, 0.001671102, 0.0035984742, 0.1650576391, 0.0058367059, 0.0040807738, 0.0928870725, 0.000132936, 0.0479163159, 0.0128213926, 0.0156118159, 0.0055771748, NA, 0.0147174501, 0.0395492518, 0.0490960392, 0.176187393, 0.2108153867, 0.0069150329, 4.82114043340968E-19, 0.0013114908, 0.002527667, 0.0004194573, 0.0024787444, 0.0012325248, NA ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0,   _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0,  _,  _,  _,  _ ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.88348474887241,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.824815839767602,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.521117957342711,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.05719073465331,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.697124684657136,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.708628392324746,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.839770659735494,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.770748413729837,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.847823255102821,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.806409907499427,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.64075651708585,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.705177280024463,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.03648406085162,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.609696506383304,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.539523889610886,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.303697882424891,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.528020181943276,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.522268328109472,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.437140891369161,  _,  _,  _,   _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.424486812934791,  _,  _,  _,   _,</t>
   </si>
 </sst>
 </file>
@@ -567,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +604,7 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -784,10 +808,10 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -844,7 +868,7 @@
         <v>5.5771748000000001E-3</v>
       </c>
       <c r="R11" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="S11">
         <v>1.47174501E-2</v>
@@ -888,7 +912,7 @@
         <v>63000000000000</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1116,7 +1140,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1197,7 @@
         <v>5.5771748000000001E-3</v>
       </c>
       <c r="R22" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="S22">
         <v>1.47174501E-2</v>
@@ -1220,79 +1244,79 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D25" s="6"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B28" s="5">
         <v>1000000000000000</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="L28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B29" s="2">
         <v>4000000000000000</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L29" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2">
         <v>63000000000000</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="L30" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1406,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1504,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="AF4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1528,7 +1552,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -1555,9 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1566,12 +1588,12 @@
         <v>0</v>
       </c>
       <c r="G1" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1585,9 +1607,9 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
         <f>IF(ISNUMBER(A2),A2*$G$1, A2)</f>
-        <v xml:space="preserve">  _</v>
+        <v>0</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:K17" si="0">IF(ISNUMBER(B2),B2*$G$1, B2)</f>
@@ -1607,15 +1629,15 @@
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M29" si="1">"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
-        <v xml:space="preserve">    _,   _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,   _,  _,  _,   _,</v>
       </c>
       <c r="T2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3">
+        <v>0.88348474887241046</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1629,9 +1651,9 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3">
         <f t="shared" ref="G3:G30" si="2">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
-        <v xml:space="preserve">  _</v>
+        <v>0.88348474887241046</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -1651,15 +1673,15 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.88348474887241,  _,  _,  _,   _,</v>
       </c>
       <c r="T3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4">
+        <v>0.82481583976760187</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1673,9 +1695,9 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G4">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.82481583976760187</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -1695,15 +1717,15 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.824815839767602,  _,  _,  _,   _,</v>
       </c>
       <c r="T4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5">
+        <v>0.52111795734271082</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1717,9 +1739,9 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.52111795734271082</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -1739,15 +1761,15 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.521117957342711,  _,  _,  _,   _,</v>
       </c>
       <c r="T5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="A6">
+        <v>1.057190734653314</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1761,9 +1783,9 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>1.057190734653314</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -1783,15 +1805,15 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  1.05719073465331,  _,  _,  _,   _,</v>
       </c>
       <c r="T6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="A7">
+        <v>0.6971246846571364</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1805,9 +1827,9 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.6971246846571364</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1827,15 +1849,15 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.697124684657136,  _,  _,  _,   _,</v>
       </c>
       <c r="T7" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
+      <c r="A8">
+        <v>0.70862839232474584</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1849,9 +1871,9 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.70862839232474584</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1871,15 +1893,15 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.708628392324746,  _,  _,  _,   _,</v>
       </c>
       <c r="T8" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="A9">
+        <v>0.83977065973549425</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1893,9 +1915,9 @@
       <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="G9" t="str">
+      <c r="G9">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.83977065973549425</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1915,18 +1937,18 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.839770659735494,  _,  _,  _,   _,</v>
       </c>
       <c r="T9" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>3.0573402278289169E-2</v>
-      </c>
-      <c r="B10">
-        <v>3.0573402278289169E-2</v>
+      <c r="A10">
+        <v>0.77074841372983727</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1939,11 +1961,11 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>1.5286701139144585E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>1.5286701139144585E-2</v>
+        <v>0.77074841372983727</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1959,18 +1981,18 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0152867011391446, 0.0152867011391446,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.770748413729837,  _,  _,  _,   _,</v>
       </c>
       <c r="T10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
+      <c r="A11">
+        <v>0.84782325510282086</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1981,13 +2003,13 @@
       <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G11">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.84782325510282086</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -2003,18 +2025,18 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,   _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.847823255102821,  _,  _,  _,   _,</v>
       </c>
       <c r="T11" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2.1108827137398572E-2</v>
-      </c>
-      <c r="B12">
-        <v>2.1108827137398572E-2</v>
+        <v>0.80640990749942665</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -2027,11 +2049,11 @@
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>1.0554413568699286E-2</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>1.0554413568699286E-2</v>
+        <v>0.80640990749942665</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -2047,21 +2069,21 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0105544135686993, 0.0105544135686993,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.806409907499427,  _,  _,  _,   _,</v>
       </c>
       <c r="T12" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5.7063444387811567E-3</v>
-      </c>
-      <c r="B13">
-        <v>5.7063444387811567E-3</v>
-      </c>
-      <c r="C13">
-        <v>5.7063444387811567E-3</v>
+        <v>0.6407565170858498</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -2071,15 +2093,15 @@
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>2.8531722193905784E-3</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>2.8531722193905784E-3</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>2.8531722193905784E-3</v>
+        <v>0.6407565170858498</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -2091,18 +2113,18 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00285317221939058, 0.00285317221939058, 0.00285317221939058,  _,   _,</v>
+        <v xml:space="preserve">  0.64075651708585,  _,  _,  _,   _,</v>
       </c>
       <c r="T13" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1.4481667457081206E-2</v>
-      </c>
-      <c r="B14">
-        <v>1.4481667457081206E-2</v>
+        <v>0.70517728002446289</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -2115,11 +2137,11 @@
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>7.2408337285406032E-3</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>7.2408337285406032E-3</v>
+        <v>0.70517728002446289</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -2135,15 +2157,15 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.0072408337285406, 0.0072408337285406,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.705177280024463,  _,  _,  _,   _,</v>
       </c>
       <c r="T14" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6.4981639798683988E-2</v>
+        <v>1.036484060851617</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -2159,7 +2181,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>3.2490819899341994E-2</v>
+        <v>1.036484060851617</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -2179,15 +2201,15 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.032490819899342,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  1.03648406085162,  _,  _,  _,   _,</v>
       </c>
       <c r="T15" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
+      <c r="A16">
+        <v>0.60969650638330419</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2201,9 +2223,9 @@
       <c r="E16" t="s">
         <v>3</v>
       </c>
-      <c r="G16" t="str">
+      <c r="G16">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.60969650638330419</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -2223,15 +2245,15 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.609696506383304,  _,  _,  _,   _,</v>
       </c>
       <c r="T16" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
+      <c r="A17">
+        <v>0.6718165277883954</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -2245,9 +2267,9 @@
       <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G17">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0.6718165277883954</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2267,21 +2289,21 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</v>
       </c>
       <c r="T17" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6.7926514832037542E-3</v>
-      </c>
-      <c r="B18">
-        <v>6.7926514832037542E-3</v>
-      </c>
-      <c r="C18">
-        <v>6.7926514832037542E-3</v>
+        <v>0.6718165277883954</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -2291,15 +2313,15 @@
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>3.3963257416018771E-3</v>
-      </c>
-      <c r="H18">
+        <v>0.6718165277883954</v>
+      </c>
+      <c r="H18" t="str">
         <f t="shared" ref="H18:H31" si="3">IF(ISNUMBER(B18),B18*$G$1, B18)</f>
-        <v>3.3963257416018771E-3</v>
-      </c>
-      <c r="I18">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I18" t="str">
         <f t="shared" ref="I18:I31" si="4">IF(ISNUMBER(C18),C18*$G$1, C18)</f>
-        <v>3.3963257416018771E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ref="J18:J31" si="5">IF(ISNUMBER(D18),D18*$G$1, D18)</f>
@@ -2311,18 +2333,18 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00339632574160188, 0.00339632574160188, 0.00339632574160188,  _,   _,</v>
+        <v xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</v>
       </c>
       <c r="T18" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1.9400287828099102E-2</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1.9400287828099102E-2</v>
+        <v>0.53952388961088593</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -2335,11 +2357,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>9.7001439140495509E-3</v>
-      </c>
-      <c r="H19">
+        <v>0.53952388961088593</v>
+      </c>
+      <c r="H19" t="str">
         <f t="shared" si="3"/>
-        <v>9.7001439140495509E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="4"/>
@@ -2355,18 +2377,18 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00970014391404955, 0.00970014391404955,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.539523889610886,  _,  _,  _,   _,</v>
       </c>
       <c r="T19" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1.8392655758024037E-2</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1.8392655758024037E-2</v>
+        <v>0.3036978824248911</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -2379,11 +2401,11 @@
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>9.1963278790120184E-3</v>
-      </c>
-      <c r="H20">
+        <v>0.3036978824248911</v>
+      </c>
+      <c r="H20" t="str">
         <f t="shared" si="3"/>
-        <v>9.1963278790120184E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="4"/>
@@ -2399,21 +2421,21 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00919632787901202, 0.00919632787901202,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.303697882424891,  _,  _,  _,   _,</v>
       </c>
       <c r="T20" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5.3143143366253523E-3</v>
-      </c>
-      <c r="B21">
-        <v>5.3143143366253523E-3</v>
-      </c>
-      <c r="C21">
-        <v>5.3143143366253523E-3</v>
+        <v>0.52802018194327649</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -2423,15 +2445,15 @@
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>2.6571571683126761E-3</v>
-      </c>
-      <c r="H21">
+        <v>0.52802018194327649</v>
+      </c>
+      <c r="H21" t="str">
         <f t="shared" si="3"/>
-        <v>2.6571571683126761E-3</v>
-      </c>
-      <c r="I21">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I21" t="str">
         <f t="shared" si="4"/>
-        <v>2.6571571683126761E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="5"/>
@@ -2443,21 +2465,21 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00265715716831268, 0.00265715716831268, 0.00265715716831268,  _,   _,</v>
+        <v xml:space="preserve">  0.528020181943276,  _,  _,  _,   _,</v>
       </c>
       <c r="T21" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4.6038719504543461E-3</v>
-      </c>
-      <c r="B22">
-        <v>4.6038719504543461E-3</v>
-      </c>
-      <c r="C22">
-        <v>4.6038719504543461E-3</v>
+        <v>0.52226832810947188</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -2467,15 +2489,15 @@
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>2.3019359752271731E-3</v>
-      </c>
-      <c r="H22">
+        <v>0.52226832810947188</v>
+      </c>
+      <c r="H22" t="str">
         <f t="shared" si="3"/>
-        <v>2.3019359752271731E-3</v>
-      </c>
-      <c r="I22">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I22" t="str">
         <f t="shared" si="4"/>
-        <v>2.3019359752271731E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="5"/>
@@ -2487,21 +2509,21 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00230193597522717, 0.00230193597522717, 0.00230193597522717,  _,   _,</v>
+        <v xml:space="preserve">  0.522268328109472,  _,  _,  _,   _,</v>
       </c>
       <c r="T22" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5.6887969608433314E-3</v>
-      </c>
-      <c r="B23">
-        <v>5.6887969608433314E-3</v>
-      </c>
-      <c r="C23">
-        <v>5.6887969608433314E-3</v>
+        <v>0.4371408913691614</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -2511,15 +2533,15 @@
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>2.8443984804216657E-3</v>
-      </c>
-      <c r="H23">
+        <v>0.4371408913691614</v>
+      </c>
+      <c r="H23" t="str">
         <f t="shared" si="3"/>
-        <v>2.8443984804216657E-3</v>
-      </c>
-      <c r="I23">
+        <v xml:space="preserve"> _</v>
+      </c>
+      <c r="I23" t="str">
         <f t="shared" si="4"/>
-        <v>2.8443984804216657E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="5"/>
@@ -2531,18 +2553,18 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00284439848042167, 0.00284439848042167, 0.00284439848042167,  _,   _,</v>
+        <v xml:space="preserve">  0.437140891369161,  _,  _,  _,   _,</v>
       </c>
       <c r="T23" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1.3283900379781735E-2</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1.3283900379781735E-2</v>
+        <v>0.4244868129347909</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -2555,11 +2577,11 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>6.6419501898908676E-3</v>
-      </c>
-      <c r="H24">
+        <v>0.4244868129347909</v>
+      </c>
+      <c r="H24" t="str">
         <f t="shared" si="3"/>
-        <v>6.6419501898908676E-3</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="4"/>
@@ -2575,15 +2597,15 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.00664195018989087, 0.00664195018989087,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.424486812934791,  _,  _,  _,   _,</v>
       </c>
       <c r="T24" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
+      <c r="A25">
+        <v>0</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -2597,9 +2619,9 @@
       <c r="E25" t="s">
         <v>3</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G25">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="3"/>
@@ -2619,15 +2641,15 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T25" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1</v>
+      <c r="A26">
+        <v>0</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -2641,9 +2663,9 @@
       <c r="E26" t="s">
         <v>3</v>
       </c>
-      <c r="G26" t="str">
+      <c r="G26">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> _</v>
+        <v>0</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="3"/>
@@ -2663,15 +2685,15 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T26" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
+      <c r="A27">
+        <v>0</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -2685,9 +2707,9 @@
       <c r="E27" t="s">
         <v>3</v>
       </c>
-      <c r="G27" t="str">
+      <c r="G27">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="3"/>
@@ -2707,15 +2729,15 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T27" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>1</v>
+      <c r="A28">
+        <v>0</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -2729,9 +2751,9 @@
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="G28" t="str">
+      <c r="G28">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> _</v>
+        <v>0</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="3"/>
@@ -2751,15 +2773,15 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T28" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
+      <c r="A29">
+        <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -2773,9 +2795,9 @@
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="G29" t="str">
+      <c r="G29">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  _</v>
+        <v>0</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="3"/>
@@ -2795,15 +2817,15 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T29" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1</v>
+      <c r="A30">
+        <v>0</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -2817,9 +2839,9 @@
       <c r="E30" t="s">
         <v>3</v>
       </c>
-      <c r="G30" t="str">
+      <c r="G30">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> _</v>
+        <v>0</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="3"/>
@@ -2839,15 +2861,15 @@
       </c>
       <c r="M30" t="str">
         <f>"  "&amp;G30&amp;", "&amp;H30&amp;", "&amp;I30&amp;", "&amp;J30&amp;", "&amp;K30&amp;","</f>
-        <v xml:space="preserve">   _,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
       </c>
       <c r="T30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1</v>
+      <c r="A31">
+        <v>0</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -2859,11 +2881,11 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" t="str">
+        <v>1</v>
+      </c>
+      <c r="G31">
         <f>IF(ISNUMBER(A31),A31*$G$1, A31)</f>
-        <v xml:space="preserve"> _</v>
+        <v>0</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="3"/>
@@ -2879,14 +2901,14 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> _ ;</v>
+        <v xml:space="preserve"> _</v>
       </c>
       <c r="M31" t="str">
         <f>"  "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;" ;"</f>
-        <v xml:space="preserve">   _,  _,  _,  _,  _ ; ;</v>
+        <v xml:space="preserve">  0,  _,  _,  _,  _ ;</v>
       </c>
       <c r="T31" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3205,7 +3227,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
init changes - fix issue causing multiple timesteps
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -17,7 +17,7 @@
     <sheet name="3D_init_changer" sheetId="1" r:id="rId3"/>
     <sheet name="2D_init_changer" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
   <si>
     <t xml:space="preserve"> Loligo_Squid_N1 =</t>
   </si>
@@ -62,9 +62,6 @@
     <t>(paste scalar here)</t>
   </si>
   <si>
-    <t xml:space="preserve">  0, 67.1800620400568, 67.169624003467, 67.2106814919619, 67.1100631326957, 67.2183511878286, 67.2072937091949, 67.2188746729358, 67.1256052351668, 0, 0, 0, 0, 67.2066000827306, 0, 67.2090784058426, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
-  </si>
-  <si>
     <t>CLA</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>XXX_N =</t>
   </si>
   <si>
-    <t xml:space="preserve">  0, 0, 286.941609468405, 0, 0, 286.924976095042, 287.06406178004, 287.161741675816, 286.982344649134, 287.115928093719, 0, 0, 286.779016476727, 287.161104132294, 0, 287.192135890684, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
-  </si>
-  <si>
     <t>QHG</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>SEE 'spring_invert_PA_scaled_Atl_boxes.xlsx' for biomass scaling</t>
   </si>
   <si>
-    <t xml:space="preserve">  0, 0.0941, 0.2295, 0.1068, 0.0282, 0.0849, 0.1489, 0.0794, 0.0494, 0, 0, 0, 0, 0.1085, 0, 0.0703, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
-  </si>
-  <si>
     <t>Scalar, also used for XXX_cover</t>
   </si>
   <si>
@@ -113,88 +104,100 @@
     <t xml:space="preserve">  0, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.088379386, 0, 0, 0, 0, 0.088379386, 0, 0.088379386, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>RCB</t>
   </si>
   <si>
     <t>CRD 06-25 p369</t>
   </si>
   <si>
-    <t xml:space="preserve">  0, 3.47237897680724E-05, 0.0166036077, 0.1179608232, 0.0042714077, 0.0006875969, 0.001671102, 0.0035984742, 0.1650576391, 0.0058367059, 0.0040807738, 0.0928870725, 0.000132936, 0.0479163159, 0.0128213926, 0.0156118159, 0.0055771748, NA, 0.0147174501, 0.0395492518, 0.0490960392, 0.176187393, 0.2108153867, 0.0069150329, 4.82114043340968E-19, 0.0013114908, 0.002527667, 0.0004194573, 0.0024787444, 0.0012325248, NA ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0,   _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0,  _,  _,  _,  _ ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.88348474887241,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.824815839767602,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.521117957342711,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1.05719073465331,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.697124684657136,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.708628392324746,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.839770659735494,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.770748413729837,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.847823255102821,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.806409907499427,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.64075651708585,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.705177280024463,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1.03648406085162,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.609696506383304,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.539523889610886,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.303697882424891,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.528020181943276,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.522268328109472,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.437140891369161,  _,  _,  _,   _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.424486812934791,  _,  _,  _,   _,</t>
+    <t xml:space="preserve">  0, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, _, _, _, _ ;</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 67.1800620400568, 67.169624003467, 67.2106814919619, 67.1100631326957, 67.2183511878286, 67.2072937091949, 67.2188746729358, 67.1256052351668, 0, 0, 0, 0, 67.2066000827306, 0, 67.2090784058426, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0.0941, 0.2295, 0.1068, 0.0282, 0.0849, 0.1489, 0.0794, 0.0494, 0, 0, 0, 0, 0.1085, 0, 0.0703, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0, 286.941609468405, 0, 0, 286.924976095042, 287.06406178004, 287.161741675816, 286.982344649134, 287.115928093719, 0, 0, 286.779016476727, 287.161104132294, 0, 287.192135890684, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.163401316, 0.088379386, 0, 0, 0, 0, 0.088379386, 0, 0.088379386, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 3.84127855690434E-05, 0.0183675464721034, 0.130492778507021, 0.00472519471964219, 0.000760646013987926, 0.00184863700704185, 0.00398076992009183, 0.182593079258607, 0.00645678751264703, 0.00451430820144239, 0.102755235586624, 0.000147058892376477, 0.053006863024428, 0.0141835153342959, 0.0172703884142705, 0.00616968427422216, 0.0162810067273881, 0.0162810067273881, 0.0437508964014742, 0.0543119181021249, 0.194905239102117, 0.233212051393307, 0, 0, 0, 0, 0, 0, 0 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0413120539948171, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0028977848000201, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00356987730842551, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0816681808693169, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00621629418047132, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0141895111622896, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0306376895364652, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.012805807845432, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00253243374269256, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0053262345418044, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00191700421617492, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0639285713586265, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00876897014481673, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00605562080749151, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00731245858568842, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.00158914584916489, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0202073681824202, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0199457993403265, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0110120510423912, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0183785957231647, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0339145663632122, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.0195010475010361, _, _, _, _,</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -292,11 +295,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -309,6 +323,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,17 +607,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD30"/>
+  <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -808,7 +826,7 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
@@ -820,96 +838,96 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>3.4723789768072398E-5</v>
+        <v>9.4100000000000003E-2</v>
       </c>
       <c r="C11">
-        <v>1.6603607699999998E-2</v>
+        <v>0.22950000000000001</v>
       </c>
       <c r="D11">
-        <v>0.1179608232</v>
+        <v>0.10680000000000001</v>
       </c>
       <c r="E11">
-        <v>4.2714077000000003E-3</v>
+        <v>2.8199999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>6.8759690000000004E-4</v>
+        <v>8.4900000000000003E-2</v>
       </c>
       <c r="G11">
-        <v>1.671102E-3</v>
+        <v>0.1489</v>
       </c>
       <c r="H11">
-        <v>3.5984742E-3</v>
+        <v>7.9399999999999998E-2</v>
       </c>
       <c r="I11">
-        <v>0.16505763909999999</v>
+        <v>4.9399999999999999E-2</v>
       </c>
       <c r="J11">
-        <v>5.8367059000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>4.0807737999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>9.2887072500000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>1.32936E-4</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>4.7916315899999999E-2</v>
+        <v>0.1085</v>
       </c>
       <c r="O11">
-        <v>1.28213926E-2</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>1.5611815899999999E-2</v>
+        <v>7.0300000000000001E-2</v>
       </c>
       <c r="Q11">
-        <v>5.5771748000000001E-3</v>
-      </c>
-      <c r="R11" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>1.47174501E-2</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>3.9549251799999997E-2</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>4.9096039199999997E-2</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>0.176187393</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>0.2108153867</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>6.9150328999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="Y11">
-        <v>4.8211404334096802E-19</v>
+        <v>0</v>
       </c>
       <c r="Z11">
-        <v>1.3114908000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="AA11">
-        <v>2.5276669999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="AB11">
-        <v>4.1945730000000003E-4</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <v>2.4787443999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <v>1.2325248000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>63000000000000</v>
+      <c r="A13" s="5">
+        <v>1000000000000000</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -924,223 +942,252 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15:AD15" si="0">$A$13*B11/20/5.7/B2</f>
-        <v>1.5617749214214083E-3</v>
+        <v>67.180062040056782</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>0.30614927859492075</v>
+        <v>67.16962400346695</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>4.6767633047506045</v>
+        <v>67.210681491961935</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.64039821794278029</v>
+        <v>67.110063132695714</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>3.429688084442075E-2</v>
+        <v>67.218351187828588</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>4.7518773033696775E-2</v>
+        <v>67.2072937091949</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="0"/>
-        <v>0.19192417297992889</v>
+        <v>67.218874672935797</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="0"/>
-        <v>14.1298465013429</v>
+        <v>67.125605235166759</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>0.18626695057124343</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>0.20090520150414479</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="0"/>
-        <v>3.2104209680850873</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="0"/>
-        <v>1.7155464900457561E-2</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="0"/>
-        <v>1.8698473626555978</v>
+        <v>67.206600082730588</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="0"/>
-        <v>0.56195333763762723</v>
+        <v>0</v>
       </c>
       <c r="P15" s="2">
         <f t="shared" si="0"/>
-        <v>0.94030032445921519</v>
+        <v>67.209078405842575</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="0"/>
-        <v>0.27216527225356729</v>
-      </c>
-      <c r="R15" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <f>$A$13*R11/20/5.7/R2</f>
+        <v>0</v>
       </c>
       <c r="S15" s="2">
         <f t="shared" si="0"/>
-        <v>1.6834458421315674</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
         <f t="shared" si="0"/>
-        <v>1.2359658368686464</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" si="0"/>
-        <v>2.7248959740064214</v>
+        <v>0</v>
       </c>
       <c r="V15" s="2">
         <f t="shared" si="0"/>
-        <v>16.136938632383174</v>
+        <v>0</v>
       </c>
       <c r="W15" s="2">
         <f t="shared" si="0"/>
-        <v>6.7565909924024945</v>
+        <v>0</v>
       </c>
       <c r="X15" s="2">
         <f t="shared" si="0"/>
-        <v>22.086070182737163</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="2">
         <f t="shared" si="0"/>
-        <v>9.0439774709140483E-16</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="2">
         <f t="shared" si="0"/>
-        <v>2.0383741272765581E-2</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="2">
         <f t="shared" si="0"/>
-        <v>7.9687749082708245E-2</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="2">
         <f t="shared" si="0"/>
-        <v>8.9041325304368198E-3</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="2">
         <f t="shared" si="0"/>
-        <v>3.4047825561724712E-2</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="2">
         <f t="shared" si="0"/>
-        <v>2.4833692685516676E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <f>IF(ISNUMBER(A15),A15,_)</f>
         <v>0</v>
       </c>
-      <c r="B16">
-        <v>9.4100000000000003E-2</v>
-      </c>
-      <c r="C16">
-        <v>0.22950000000000001</v>
-      </c>
-      <c r="D16">
-        <v>0.10680000000000001</v>
-      </c>
-      <c r="E16">
-        <v>2.8199999999999999E-2</v>
-      </c>
-      <c r="F16">
-        <v>8.4900000000000003E-2</v>
-      </c>
-      <c r="G16">
-        <v>0.1489</v>
-      </c>
-      <c r="H16">
-        <v>7.9399999999999998E-2</v>
-      </c>
-      <c r="I16">
-        <v>4.9399999999999999E-2</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0.1085</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>7.0300000000000001E-2</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>0</v>
-      </c>
-      <c r="AD16">
+      <c r="B16" s="8">
+        <f>IF(ISNUMBER(B15),B15,_)</f>
+        <v>67.180062040056782</v>
+      </c>
+      <c r="C16" s="8">
+        <f>IF(ISNUMBER(C15),C15,_)</f>
+        <v>67.16962400346695</v>
+      </c>
+      <c r="D16" s="8">
+        <f>IF(ISNUMBER(D15),D15,_)</f>
+        <v>67.210681491961935</v>
+      </c>
+      <c r="E16" s="8">
+        <f>IF(ISNUMBER(E15),E15,_)</f>
+        <v>67.110063132695714</v>
+      </c>
+      <c r="F16" s="8">
+        <f>IF(ISNUMBER(F15),F15,_)</f>
+        <v>67.218351187828588</v>
+      </c>
+      <c r="G16" s="8">
+        <f>IF(ISNUMBER(G15),G15,_)</f>
+        <v>67.2072937091949</v>
+      </c>
+      <c r="H16" s="8">
+        <f>IF(ISNUMBER(H15),H15,_)</f>
+        <v>67.218874672935797</v>
+      </c>
+      <c r="I16" s="8">
+        <f>IF(ISNUMBER(I15),I15,_)</f>
+        <v>67.125605235166759</v>
+      </c>
+      <c r="J16" s="8">
+        <f>IF(ISNUMBER(J15),J15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
+        <f>IF(ISNUMBER(K15),K15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <f>IF(ISNUMBER(L15),L15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="8">
+        <f>IF(ISNUMBER(M15),M15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <f>IF(ISNUMBER(N15),N15,_)</f>
+        <v>67.206600082730588</v>
+      </c>
+      <c r="O16" s="8">
+        <f>IF(ISNUMBER(O15),O15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
+        <f>IF(ISNUMBER(P15),P15,_)</f>
+        <v>67.209078405842575</v>
+      </c>
+      <c r="Q16" s="8">
+        <f>IF(ISNUMBER(Q15),Q15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="8">
+        <f>IF(ISNUMBER(R15),R15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="8">
+        <f>IF(ISNUMBER(S15),S15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="8">
+        <f>IF(ISNUMBER(T15),T15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="8">
+        <f>IF(ISNUMBER(U15),U15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="8">
+        <f>IF(ISNUMBER(V15),V15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="8">
+        <f>IF(ISNUMBER(W15),W15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="8">
+        <f>IF(ISNUMBER(X15),X15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="8">
+        <f>IF(ISNUMBER(Y15),Y15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="8">
+        <f>IF(ISNUMBER(Z15),Z15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="8">
+        <f>IF(ISNUMBER(AA15),AA15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="8">
+        <f>IF(ISNUMBER(AB15),AB15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="8">
+        <f>IF(ISNUMBER(AC15),AC15,_)</f>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="8">
+        <f>IF(ISNUMBER(AD15),AD15,_)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>"  "&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;G16&amp;", "&amp;H16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;", "&amp;P16&amp;", "&amp;Q16&amp;", "&amp;R16&amp;", "&amp;S16&amp;", "&amp;T16&amp;", "&amp;U16&amp;", "&amp;V16&amp;", "&amp;W16&amp;", "&amp;X16&amp;", "&amp;Y16&amp;", "&amp;Z16&amp;", "&amp;AA16&amp;", "&amp;AB16&amp;", "&amp;AC16&amp;", "&amp;AD16&amp;", "&amp;R16&amp;" ;"</f>
-        <v xml:space="preserve">  0, 0.0941, 0.2295, 0.1068, 0.0282, 0.0849, 0.1489, 0.0794, 0.0494, 0, 0, 0, 0, 0.1085, 0, 0.0703, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</v>
+        <f>"  "&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;G16&amp;", "&amp;H16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;", "&amp;P16&amp;", "&amp;Q16&amp;", "&amp;R16&amp;", "&amp;S16&amp;", "&amp;T16&amp;", "&amp;U16&amp;", "&amp;V16&amp;", "&amp;W16&amp;", "&amp;X16&amp;", "&amp;Y16&amp;", "&amp;Z16&amp;", "&amp;AA16&amp;", "&amp;AB16&amp;", "&amp;AC16&amp;", "&amp;AD16&amp;" ;"</f>
+        <v xml:space="preserve">  0, 67.1800620400568, 67.169624003467, 67.2106814919619, 67.1100631326957, 67.2183511878286, 67.2072937091949, 67.2188746729358, 67.1256052351668, 0, 0, 0, 0, 67.2066000827306, 0, 67.2090784058426, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>24</v>
+      <c r="A20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1149,174 +1196,179 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>3.4723789768072398E-5</v>
+        <v>3.8412785569043447E-5</v>
       </c>
       <c r="C22">
-        <v>1.6603607699999998E-2</v>
+        <v>1.8367546472103407E-2</v>
       </c>
       <c r="D22">
-        <v>0.1179608232</v>
+        <v>0.13049277850702132</v>
       </c>
       <c r="E22">
-        <v>4.2714077000000003E-3</v>
+        <v>4.7251947196421864E-3</v>
       </c>
       <c r="F22">
-        <v>6.8759690000000004E-4</v>
+        <v>7.6064601398792629E-4</v>
       </c>
       <c r="G22">
-        <v>1.671102E-3</v>
+        <v>1.8486370070418463E-3</v>
       </c>
       <c r="H22">
-        <v>3.5984742E-3</v>
+        <v>3.9807699200918329E-3</v>
       </c>
       <c r="I22">
-        <v>0.16505763909999999</v>
+        <v>0.18259307925860729</v>
       </c>
       <c r="J22">
-        <v>5.8367059000000001E-3</v>
+        <v>6.4567875126470345E-3</v>
       </c>
       <c r="K22">
-        <v>4.0807737999999996E-3</v>
+        <v>4.5143082014423895E-3</v>
       </c>
       <c r="L22">
-        <v>9.2887072500000001E-2</v>
+        <v>0.10275523558662426</v>
       </c>
       <c r="M22">
-        <v>1.32936E-4</v>
+        <v>1.4705889237647663E-4</v>
       </c>
       <c r="N22">
-        <v>4.7916315899999999E-2</v>
+        <v>5.3006863024427968E-2</v>
       </c>
       <c r="O22">
-        <v>1.28213926E-2</v>
+        <v>1.4183515334295856E-2</v>
       </c>
       <c r="P22">
-        <v>1.5611815899999999E-2</v>
+        <v>1.7270388414270525E-2</v>
       </c>
       <c r="Q22">
-        <v>5.5771748000000001E-3</v>
-      </c>
-      <c r="R22" t="s">
-        <v>28</v>
+        <v>6.169684274222164E-3</v>
+      </c>
+      <c r="R22">
+        <v>1.6281006727388105E-2</v>
       </c>
       <c r="S22">
-        <v>1.47174501E-2</v>
+        <v>1.6281006727388105E-2</v>
       </c>
       <c r="T22">
-        <v>3.9549251799999997E-2</v>
+        <v>4.3750896401474199E-2</v>
       </c>
       <c r="U22">
-        <v>4.9096039199999997E-2</v>
+        <v>5.4311918102124913E-2</v>
       </c>
       <c r="V22">
-        <v>0.176187393</v>
+        <v>0.19490523910211674</v>
       </c>
       <c r="W22">
-        <v>0.2108153867</v>
+        <v>0.23321205139330659</v>
       </c>
       <c r="X22">
-        <v>6.9150328999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="Y22">
-        <v>4.8211404334096802E-19</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <v>1.3114908000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="AA22">
-        <v>2.5276669999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="AB22">
-        <v>4.1945730000000003E-4</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <v>2.4787443999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <v>1.2325248000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>"  "&amp;A22&amp;", "&amp;B22&amp;", "&amp;C22&amp;", "&amp;D22&amp;", "&amp;E22&amp;", "&amp;F22&amp;", "&amp;G22&amp;", "&amp;H22&amp;", "&amp;I22&amp;", "&amp;J22&amp;", "&amp;K22&amp;", "&amp;L22&amp;", "&amp;M22&amp;", "&amp;N22&amp;", "&amp;O22&amp;", "&amp;P22&amp;", "&amp;Q22&amp;", "&amp;R22&amp;", "&amp;S22&amp;", "&amp;T22&amp;", "&amp;U22&amp;", "&amp;V22&amp;", "&amp;W22&amp;", "&amp;X22&amp;", "&amp;Y22&amp;", "&amp;Z22&amp;", "&amp;AA22&amp;", "&amp;AB22&amp;", "&amp;AC22&amp;", "&amp;AD22&amp;", "&amp;R22&amp;" ;"</f>
-        <v xml:space="preserve">  0, 3.47237897680724E-05, 0.0166036077, 0.1179608232, 0.0042714077, 0.0006875969, 0.001671102, 0.0035984742, 0.1650576391, 0.0058367059, 0.0040807738, 0.0928870725, 0.000132936, 0.0479163159, 0.0128213926, 0.0156118159, 0.0055771748, NA, 0.0147174501, 0.0395492518, 0.0490960392, 0.176187393, 0.2108153867, 0.0069150329, 4.82114043340968E-19, 0.0013114908, 0.002527667, 0.0004194573, 0.0024787444, 0.0012325248, NA ;</v>
+        <f>"  "&amp;A22&amp;", "&amp;B22&amp;", "&amp;C22&amp;", "&amp;D22&amp;", "&amp;E22&amp;", "&amp;F22&amp;", "&amp;G22&amp;", "&amp;H22&amp;", "&amp;I22&amp;", "&amp;J22&amp;", "&amp;K22&amp;", "&amp;L22&amp;", "&amp;M22&amp;", "&amp;N22&amp;", "&amp;O22&amp;", "&amp;P22&amp;", "&amp;Q22&amp;", "&amp;R22&amp;", "&amp;S22&amp;", "&amp;T22&amp;", "&amp;U22&amp;", "&amp;V22&amp;", "&amp;W22&amp;", "&amp;X22&amp;", "&amp;Y22&amp;", "&amp;Z22&amp;", "&amp;AA22&amp;", "&amp;AB22&amp;", "&amp;AC22&amp;", "&amp;AD22&amp;" ;"</f>
+        <v xml:space="preserve">  0, 3.84127855690434E-05, 0.0183675464721034, 0.130492778507021, 0.00472519471964219, 0.000760646013987926, 0.00184863700704185, 0.00398076992009183, 0.182593079258607, 0.00645678751264703, 0.00451430820144239, 0.102755235586624, 0.000147058892376477, 0.053006863024428, 0.0141835153342959, 0.0172703884142705, 0.00616968427422216, 0.0162810067273881, 0.0162810067273881, 0.0437508964014742, 0.0543119181021249, 0.194905239102117, 0.233212051393307, 0, 0, 0, 0, 0, 0, 0 ;</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="6"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E27" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="5">
         <v>1000000000000000</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
       </c>
       <c r="L28" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2">
         <v>4000000000000000</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L29" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2">
         <v>63000000000000</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="L30" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="AF4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1552,7 +1604,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -1579,7 +1631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1592,20 +1646,20 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <f>IF(ISNUMBER(A2),A2*$G$1, A2)</f>
@@ -1613,1275 +1667,1275 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:K17" si="0">IF(ISNUMBER(B2),B2*$G$1, B2)</f>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M29" si="1">"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
-        <v xml:space="preserve">  0,   _,  _,  _,   _,</v>
+        <f>"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.88348474887241046</v>
+      <c r="A3" s="9">
+        <v>4.1312053994817056E-2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G30" si="2">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
-        <v>0.88348474887241046</v>
+        <f t="shared" ref="G3:G30" si="1">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
+        <v>4.1312053994817056E-2</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.88348474887241,  _,  _,  _,   _,</v>
+        <f t="shared" ref="M3:M31" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
+        <v xml:space="preserve">  0.0413120539948171, _, _, _, _,</v>
       </c>
       <c r="T3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.82481583976760187</v>
+      <c r="A4" s="9">
+        <v>2.8977848000200971E-3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G4">
+        <f t="shared" si="1"/>
+        <v>2.8977848000200971E-3</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M4" t="str">
         <f t="shared" si="2"/>
-        <v>0.82481583976760187</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.824815839767602,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0028977848000201, _, _, _, _,</v>
       </c>
       <c r="T4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.52111795734271082</v>
+      <c r="A5" s="9">
+        <v>3.5698773084255116E-3</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G5">
+        <f t="shared" si="1"/>
+        <v>3.5698773084255116E-3</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="2"/>
-        <v>0.52111795734271082</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.521117957342711,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00356987730842551, _, _, _, _,</v>
       </c>
       <c r="T5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.057190734653314</v>
+      <c r="A6" s="9">
+        <v>8.1668180869316875E-2</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G6">
+        <f t="shared" si="1"/>
+        <v>8.1668180869316875E-2</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="2"/>
-        <v>1.057190734653314</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  1.05719073465331,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0816681808693169, _, _, _, _,</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.6971246846571364</v>
+      <c r="A7" s="9">
+        <v>6.2162941804713235E-3</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G7">
+        <f t="shared" si="1"/>
+        <v>6.2162941804713235E-3</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v>0.6971246846571364</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.697124684657136,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00621629418047132, _, _, _, _,</v>
       </c>
       <c r="T7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.70862839232474584</v>
+      <c r="A8" s="9">
+        <v>1.4189511162289553E-2</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1.4189511162289553E-2</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v>0.70862839232474584</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.708628392324746,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0141895111622896, _, _, _, _,</v>
       </c>
       <c r="T8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.83977065973549425</v>
+      <c r="A9" s="9">
+        <v>3.063768953646516E-2</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G9">
+        <f t="shared" si="1"/>
+        <v>3.063768953646516E-2</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v>0.83977065973549425</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.839770659735494,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0306376895364652, _, _, _, _,</v>
       </c>
       <c r="T9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.77074841372983727</v>
+      <c r="A10" s="9">
+        <v>1.2805807845432044E-2</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1.2805807845432044E-2</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="2"/>
-        <v>0.77074841372983727</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.770748413729837,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.012805807845432, _, _, _, _,</v>
       </c>
       <c r="T10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.84782325510282086</v>
+      <c r="A11" s="9">
+        <v>2.5324337426925574E-3</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2.5324337426925574E-3</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M11" t="str">
         <f t="shared" si="2"/>
-        <v>0.84782325510282086</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.847823255102821,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00253243374269256, _, _, _, _,</v>
       </c>
       <c r="T11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0.80640990749942665</v>
+      <c r="A12" s="9">
+        <v>5.3262345418043982E-3</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G12">
+        <f t="shared" si="1"/>
+        <v>5.3262345418043982E-3</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v>0.80640990749942665</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.806409907499427,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0053262345418044, _, _, _, _,</v>
       </c>
       <c r="T12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.6407565170858498</v>
+      <c r="A13" s="9">
+        <v>1.9170042161749171E-3</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1.9170042161749171E-3</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v>0.6407565170858498</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.64075651708585,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00191700421617492, _, _, _, _,</v>
       </c>
       <c r="T13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.70517728002446289</v>
+      <c r="A14" s="9">
+        <v>6.3928571358626465E-2</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G14">
+        <f t="shared" si="1"/>
+        <v>6.3928571358626465E-2</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v>0.70517728002446289</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.705177280024463,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.0639285713586265, _, _, _, _,</v>
       </c>
       <c r="T14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1.036484060851617</v>
+      <c r="A15" s="9">
+        <v>8.7689701448167272E-3</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G15">
+        <f t="shared" si="1"/>
+        <v>8.7689701448167272E-3</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v>1.036484060851617</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  1.03648406085162,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00876897014481673, _, _, _, _,</v>
       </c>
       <c r="T15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0.60969650638330419</v>
+      <c r="A16" s="9">
+        <v>6.055620807491514E-3</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G16">
+        <f t="shared" si="1"/>
+        <v>6.055620807491514E-3</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="2"/>
-        <v>0.60969650638330419</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.609696506383304,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00605562080749151, _, _, _, _,</v>
       </c>
       <c r="T16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0.6718165277883954</v>
+      <c r="A17" s="9">
+        <v>7.3124585856884187E-3</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G17">
+        <f t="shared" si="1"/>
+        <v>7.3124585856884187E-3</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="2"/>
-        <v>0.6718165277883954</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> _</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  _</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</v>
+        <v xml:space="preserve">  0.00731245858568842, _, _, _, _,</v>
       </c>
       <c r="T17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0.6718165277883954</v>
+      <c r="A18" s="9">
+        <v>1.5891458491648861E-3</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
-        <v>0.6718165277883954</v>
+        <f t="shared" si="1"/>
+        <v>1.5891458491648861E-3</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" ref="H18:H31" si="3">IF(ISNUMBER(B18),B18*$G$1, B18)</f>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ref="I18:I31" si="4">IF(ISNUMBER(C18),C18*$G$1, C18)</f>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ref="J18:J31" si="5">IF(ISNUMBER(D18),D18*$G$1, D18)</f>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" ref="K18:K31" si="6">IF(ISNUMBER(E18),E18*$G$1, E18)</f>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.00158914584916489, _, _, _, _,</v>
+      </c>
+      <c r="T18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>2.0207368182420152E-2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.671816527788395,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0.53952388961088593</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="2"/>
-        <v>0.53952388961088593</v>
+        <v>2.0207368182420152E-2</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0202073681824202, _, _, _, _,</v>
+      </c>
+      <c r="T19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>1.9945799340326521E-2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.539523889610886,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0.3036978824248911</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="2"/>
-        <v>0.3036978824248911</v>
+        <v>1.9945799340326521E-2</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0199457993403265, _, _, _, _,</v>
+      </c>
+      <c r="T20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>1.1012051042391247E-2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.303697882424891,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0.52802018194327649</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>0.52802018194327649</v>
+        <v>1.1012051042391247E-2</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0110120510423912, _, _, _, _,</v>
+      </c>
+      <c r="T21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>1.8378595723164685E-2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.528020181943276,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0.52226832810947188</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="2"/>
-        <v>0.52226832810947188</v>
+        <v>1.8378595723164685E-2</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0183785957231647, _, _, _, _,</v>
+      </c>
+      <c r="T22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>3.3914566363212231E-2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.522268328109472,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0.4371408913691614</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="2"/>
-        <v>0.4371408913691614</v>
+        <v>3.3914566363212231E-2</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M23" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0339145663632122, _, _, _, _,</v>
+      </c>
+      <c r="T23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>1.9501047501036085E-2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.437140891369161,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0.4244868129347909</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="2"/>
-        <v>0.4244868129347909</v>
+        <v>1.9501047501036085E-2</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M24" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.0195010475010361, _, _, _, _,</v>
+      </c>
+      <c r="T24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0.424486812934791,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M25" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
+      </c>
+      <c r="T25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M26" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
+      </c>
+      <c r="T26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M27" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
+      </c>
+      <c r="T27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M28" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
+      </c>
+      <c r="T28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
+      </c>
+      <c r="T29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
-      </c>
-      <c r="T29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  _</v>
+        <v>_</v>
       </c>
       <c r="M30" t="str">
-        <f>"  "&amp;G30&amp;", "&amp;H30&amp;", "&amp;I30&amp;", "&amp;J30&amp;", "&amp;K30&amp;","</f>
-        <v xml:space="preserve">  0,  _,  _,  _,   _,</v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, _, _, _, _,</v>
       </c>
       <c r="T30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="9">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <f>IF(ISNUMBER(A31),A31*$G$1, A31)</f>
@@ -2889,26 +2943,26 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> _</v>
+        <v>_</v>
       </c>
       <c r="M31" t="str">
         <f>"  "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;" ;"</f>
-        <v xml:space="preserve">  0,  _,  _,  _,  _ ;</v>
+        <v xml:space="preserve">  0, _, _, _, _ ;</v>
       </c>
       <c r="T31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
init changes - fix phytoplankton
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="2D calc" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="3D_init_changer" sheetId="1" r:id="rId3"/>
-    <sheet name="2D_init_changer" sheetId="2" r:id="rId4"/>
+    <sheet name="3D_surfOnly" sheetId="5" r:id="rId1"/>
+    <sheet name="2D calc" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="3D_init_changer" sheetId="1" r:id="rId4"/>
+    <sheet name="2D_init_changer" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="77">
   <si>
     <t xml:space="preserve"> Loligo_Squid_N1 =</t>
   </si>
@@ -134,77 +135,137 @@
     <t xml:space="preserve">  0, 3.84127855690434E-05, 0.0183675464721034, 0.130492778507021, 0.00472519471964219, 0.000760646013987926, 0.00184863700704185, 0.00398076992009183, 0.182593079258607, 0.00645678751264703, 0.00451430820144239, 0.102755235586624, 0.000147058892376477, 0.053006863024428, 0.0141835153342959, 0.0172703884142705, 0.00616968427422216, 0.0162810067273881, 0.0162810067273881, 0.0437508964014742, 0.0543119181021249, 0.194905239102117, 0.233212051393307, 0, 0, 0, 0, 0, 0, 0 ;</t>
   </si>
   <si>
-    <t xml:space="preserve">  0.0413120539948171, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0028977848000201, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00356987730842551, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0816681808693169, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00621629418047132, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0141895111622896, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0306376895364652, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.012805807845432, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00253243374269256, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0053262345418044, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00191700421617492, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0639285713586265, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00876897014481673, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00605562080749151, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00731245858568842, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.00158914584916489, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0202073681824202, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0199457993403265, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0110120510423912, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0183785957231647, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0339145663632122, _, _, _, _,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  0.0195010475010361, _, _, _, _,</t>
+    <t xml:space="preserve">  0, 0, 0, 0, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.171, 0.171, 0.171, 0.171, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.076, 0.076, 0.076, 0.076, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.05, 0.05, 0.05, 0.05, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.288, 0.288, 0.288, 0.288, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.077, 0.077, 0.077, 0.077, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.046, 0.046, 0.046, 0.046, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.108, 0.108, 0.108, 0.108, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.047, 0.047, 0.047, 0.047, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.073, 0.073, 0.073, 0.073, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.053, 0.053, 0.053, 0.053, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.02, 0.02, 0.02, 0.02, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.051, 0.051, 0.051, 0.051, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.174, 0.174, 0.174, 0.174, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.022, 0.022, 0.022, 0.022, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.045, 0.045, 0.045, 0.045, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.089, 0.089, 0.089, 0.089, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.029, 0.029, 0.029, 0.029, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.008, 0.008, 0.008, 0.008, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0, 0, 0, 0, _ ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.299, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.166, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.104, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.348, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.167, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.103, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.138, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.175, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.136, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.131, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.112, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.128, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.175, _, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.125, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.117, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.09, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.069, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.08, _, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.123, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.12, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, _, 0.142, _, _,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _, 0.109, _, _, _,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +295,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -310,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -327,6 +395,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,6 +676,1375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>IF(ISNUMBER(A2),A2*$G$1, A2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:K17" si="0">IF(ISNUMBER(B2),B2*$G$1, B2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M2" t="str">
+        <f>"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="B3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:K31" si="1">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M31" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
+        <v xml:space="preserve">  0.299, _, _, _, _,</v>
+      </c>
+      <c r="T3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="B4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.166, _, _, _, _,</v>
+      </c>
+      <c r="T4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.104</v>
+      </c>
+      <c r="B5">
+        <v>0.104</v>
+      </c>
+      <c r="C5">
+        <v>0.104</v>
+      </c>
+      <c r="D5">
+        <v>0.104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.104</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.104, _, _,</v>
+      </c>
+      <c r="T5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="B6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.348, _, _, _, _,</v>
+      </c>
+      <c r="T6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="B7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.167, _, _, _,</v>
+      </c>
+      <c r="T7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="B8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.103, _, _, _,</v>
+      </c>
+      <c r="T8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="B9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.138, _, _, _, _,</v>
+      </c>
+      <c r="T9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.175, _, _, _,</v>
+      </c>
+      <c r="T10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="B11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="10">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.136, _, _, _,</v>
+      </c>
+      <c r="T11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="B12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="10">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.131, _, _, _,</v>
+      </c>
+      <c r="T12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.112</v>
+      </c>
+      <c r="B13">
+        <v>0.112</v>
+      </c>
+      <c r="C13">
+        <v>0.112</v>
+      </c>
+      <c r="D13">
+        <v>0.112</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="10">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.112</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.112, _, _,</v>
+      </c>
+      <c r="T13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.128</v>
+      </c>
+      <c r="B14">
+        <v>0.128</v>
+      </c>
+      <c r="C14">
+        <v>0.128</v>
+      </c>
+      <c r="D14">
+        <v>0.128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="10">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.128</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.128, _, _, _,</v>
+      </c>
+      <c r="T14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B15">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="10">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0.175, _, _, _, _,</v>
+      </c>
+      <c r="T15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.125</v>
+      </c>
+      <c r="B16">
+        <v>0.125</v>
+      </c>
+      <c r="C16">
+        <v>0.125</v>
+      </c>
+      <c r="D16">
+        <v>0.125</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="10">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.125, _, _,</v>
+      </c>
+      <c r="T16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="B17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="C17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="10">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>_</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.117, _, _, _,</v>
+      </c>
+      <c r="T17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.09</v>
+      </c>
+      <c r="B18">
+        <v>0.09</v>
+      </c>
+      <c r="C18">
+        <v>0.09</v>
+      </c>
+      <c r="D18">
+        <v>0.09</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="10">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="J18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.09, _, _,</v>
+      </c>
+      <c r="T18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="B19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="D19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="10">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.069, _, _, _,</v>
+      </c>
+      <c r="T19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.08</v>
+      </c>
+      <c r="B20">
+        <v>0.08</v>
+      </c>
+      <c r="C20">
+        <v>0.08</v>
+      </c>
+      <c r="D20">
+        <v>0.08</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="10">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.08, _, _, _,</v>
+      </c>
+      <c r="T20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.123</v>
+      </c>
+      <c r="B21">
+        <v>0.123</v>
+      </c>
+      <c r="C21">
+        <v>0.123</v>
+      </c>
+      <c r="D21">
+        <v>0.123</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="10">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0.123</v>
+      </c>
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.123, _, _,</v>
+      </c>
+      <c r="T21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.12</v>
+      </c>
+      <c r="B22">
+        <v>0.12</v>
+      </c>
+      <c r="C22">
+        <v>0.12</v>
+      </c>
+      <c r="D22">
+        <v>0.12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="10">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.12, _, _,</v>
+      </c>
+      <c r="T22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="B23">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="D23">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="10">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="J23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, _, 0.142, _, _,</v>
+      </c>
+      <c r="T23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.109</v>
+      </c>
+      <c r="B24">
+        <v>0.109</v>
+      </c>
+      <c r="C24">
+        <v>0.109</v>
+      </c>
+      <c r="D24">
+        <v>0.109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="10">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0.109</v>
+      </c>
+      <c r="I24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  _, 0.109, _, _, _,</v>
+      </c>
+      <c r="T24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="10">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="10">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10">
+        <v>25</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="10">
+        <v>26</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="10">
+        <v>27</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="10">
+        <v>28</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
+      </c>
+      <c r="T30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="10">
+        <v>29</v>
+      </c>
+      <c r="G31">
+        <f>IF(ISNUMBER(A31),A31*$G$1, A31)</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="H31:K44" si="3">IF(ISNUMBER(C31),C31*$G$1, C31)</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="M31" t="str">
+        <f>"  "&amp;G31&amp;", "&amp;H31&amp;", "&amp;I31&amp;", "&amp;J31&amp;", "&amp;K31&amp;" ;"</f>
+        <v xml:space="preserve">  0, 0, 0, 0, _ ;</v>
+      </c>
+      <c r="T31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -1376,7 +2814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AF17"/>
   <sheetViews>
@@ -1627,11 +3065,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
@@ -1646,17 +3084,17 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -1665,17 +3103,17 @@
         <f>IF(ISNUMBER(A2),A2*$G$1, A2)</f>
         <v>0</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2">
         <f t="shared" ref="H2:K17" si="0">IF(ISNUMBER(B2),B2*$G$1, B2)</f>
-        <v>_</v>
-      </c>
-      <c r="I2" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J2" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" si="0"/>
@@ -1683,43 +3121,43 @@
       </c>
       <c r="M2" t="str">
         <f>"  "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","</f>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>4.1312053994817056E-2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
+      <c r="A3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="B3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.17100000000000001</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G30" si="1">IF(ISNUMBER(A3),A3*$G$1, A3)</f>
-        <v>4.1312053994817056E-2</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>0.17100000000000001</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
@@ -1727,43 +3165,43 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" ref="M3:M31" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
-        <v xml:space="preserve">  0.0413120539948171, _, _, _, _,</v>
+        <v xml:space="preserve">  0.171, 0.171, 0.171, 0.171, _,</v>
       </c>
       <c r="T3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>2.8977848000200971E-3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
+      <c r="A4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="B4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D4">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>2.8977848000200971E-3</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -1771,43 +3209,43 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0028977848000201, _, _, _, _,</v>
+        <v xml:space="preserve">  0.076, 0.076, 0.076, 0.076, _,</v>
       </c>
       <c r="T4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>3.5698773084255116E-3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
+      <c r="A5">
+        <v>0.05</v>
+      </c>
+      <c r="B5">
+        <v>0.05</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>0.05</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>3.5698773084255116E-3</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.05</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -1815,43 +3253,43 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00356987730842551, _, _, _, _,</v>
+        <v xml:space="preserve">  0.05, 0.05, 0.05, 0.05, _,</v>
       </c>
       <c r="T5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>8.1668180869316875E-2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
+      <c r="A6">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="B6">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.28799999999999998</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>8.1668180869316875E-2</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.28799999999999998</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -1859,43 +3297,43 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0816681808693169, _, _, _, _,</v>
+        <v xml:space="preserve">  0.288, 0.288, 0.288, 0.288, _,</v>
       </c>
       <c r="T6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>6.2162941804713235E-3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
+      <c r="A7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="B7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>6.2162941804713235E-3</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -1903,43 +3341,43 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00621629418047132, _, _, _, _,</v>
+        <v xml:space="preserve">  0.077, 0.077, 0.077, 0.077, _,</v>
       </c>
       <c r="T7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>1.4189511162289553E-2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
+      <c r="A8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="B8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>1.4189511162289553E-2</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -1947,43 +3385,43 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0141895111622896, _, _, _, _,</v>
+        <v xml:space="preserve">  0.046, 0.046, 0.046, 0.046, _,</v>
       </c>
       <c r="T8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>3.063768953646516E-2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
+      <c r="A9">
+        <v>0.108</v>
+      </c>
+      <c r="B9">
+        <v>0.108</v>
+      </c>
+      <c r="C9">
+        <v>0.108</v>
+      </c>
+      <c r="D9">
+        <v>0.108</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>3.063768953646516E-2</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.108</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.108</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.108</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.108</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -1991,43 +3429,43 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0306376895364652, _, _, _, _,</v>
+        <v xml:space="preserve">  0.108, 0.108, 0.108, 0.108, _,</v>
       </c>
       <c r="T9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>1.2805807845432044E-2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
+      <c r="A10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D10">
+        <v>4.7E-2</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>1.2805807845432044E-2</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>4.7E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -2035,43 +3473,43 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.012805807845432, _, _, _, _,</v>
+        <v xml:space="preserve">  0.047, 0.047, 0.047, 0.047, _,</v>
       </c>
       <c r="T10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>2.5324337426925574E-3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
+      <c r="A11">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B11">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C11">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="D11">
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>2.5324337426925574E-3</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -2079,43 +3517,43 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00253243374269256, _, _, _, _,</v>
+        <v xml:space="preserve">  0.073, 0.073, 0.073, 0.073, _,</v>
       </c>
       <c r="T11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>5.3262345418043982E-3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
+      <c r="A12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="B12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D12">
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>5.3262345418043982E-3</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -2123,43 +3561,43 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0053262345418044, _, _, _, _,</v>
+        <v xml:space="preserve">  0.053, 0.053, 0.053, 0.053, _,</v>
       </c>
       <c r="T12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>1.9170042161749171E-3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
+      <c r="A13">
+        <v>0.02</v>
+      </c>
+      <c r="B13">
+        <v>0.02</v>
+      </c>
+      <c r="C13">
+        <v>0.02</v>
+      </c>
+      <c r="D13">
+        <v>0.02</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>1.9170042161749171E-3</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.02</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -2167,43 +3605,43 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00191700421617492, _, _, _, _,</v>
+        <v xml:space="preserve">  0.02, 0.02, 0.02, 0.02, _,</v>
       </c>
       <c r="T13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>6.3928571358626465E-2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
+      <c r="A14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="B14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>6.3928571358626465E-2</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -2211,43 +3649,43 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0639285713586265, _, _, _, _,</v>
+        <v xml:space="preserve">  0.051, 0.051, 0.051, 0.051, _,</v>
       </c>
       <c r="T14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>8.7689701448167272E-3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
+      <c r="A15">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="B15">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.17399999999999999</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>8.7689701448167272E-3</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.17399999999999999</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -2255,43 +3693,43 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00876897014481673, _, _, _, _,</v>
+        <v xml:space="preserve">  0.174, 0.174, 0.174, 0.174, _,</v>
       </c>
       <c r="T15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>6.055620807491514E-3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
+      <c r="A16">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="B16">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C16">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D16">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>6.055620807491514E-3</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -2299,43 +3737,43 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00605562080749151, _, _, _, _,</v>
+        <v xml:space="preserve">  0.022, 0.022, 0.022, 0.022, _,</v>
       </c>
       <c r="T16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>7.3124585856884187E-3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
+      <c r="A17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D17">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>7.3124585856884187E-3</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>_</v>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -2343,43 +3781,43 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00731245858568842, _, _, _, _,</v>
+        <v xml:space="preserve">  0.045, 0.045, 0.045, 0.045, _,</v>
       </c>
       <c r="T17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>1.5891458491648861E-3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
+      <c r="A18">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="B18">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C18">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>1.5891458491648861E-3</v>
-      </c>
-      <c r="H18" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H18">
         <f t="shared" ref="H18:H31" si="3">IF(ISNUMBER(B18),B18*$G$1, B18)</f>
-        <v>_</v>
-      </c>
-      <c r="I18" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I18">
         <f t="shared" ref="I18:I31" si="4">IF(ISNUMBER(C18),C18*$G$1, C18)</f>
-        <v>_</v>
-      </c>
-      <c r="J18" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J18">
         <f t="shared" ref="J18:J31" si="5">IF(ISNUMBER(D18),D18*$G$1, D18)</f>
-        <v>_</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" ref="K18:K31" si="6">IF(ISNUMBER(E18),E18*$G$1, E18)</f>
@@ -2387,43 +3825,43 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.00158914584916489, _, _, _, _,</v>
+        <v xml:space="preserve">  0.022, 0.022, 0.022, 0.022, _,</v>
       </c>
       <c r="T18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>2.0207368182420152E-2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
+      <c r="A19">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="B19">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C19">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D19">
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>2.0207368182420152E-2</v>
-      </c>
-      <c r="H19" t="str">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I19" t="str">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J19" t="str">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="6"/>
@@ -2431,43 +3869,43 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0202073681824202, _, _, _, _,</v>
+        <v xml:space="preserve">  0.089, 0.089, 0.089, 0.089, _,</v>
       </c>
       <c r="T19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>1.9945799340326521E-2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
+      <c r="A20">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="B20">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C20">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D20">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>1.9945799340326521E-2</v>
-      </c>
-      <c r="H20" t="str">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I20" t="str">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J20" t="str">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="6"/>
@@ -2475,43 +3913,43 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0199457993403265, _, _, _, _,</v>
+        <v xml:space="preserve">  0.029, 0.029, 0.029, 0.029, _,</v>
       </c>
       <c r="T20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>1.1012051042391247E-2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
+      <c r="A21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="B21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>1.1012051042391247E-2</v>
-      </c>
-      <c r="H21" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I21" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J21" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="6"/>
@@ -2519,43 +3957,43 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0110120510423912, _, _, _, _,</v>
+        <v xml:space="preserve">  0.022, 0.022, 0.022, 0.022, _,</v>
       </c>
       <c r="T21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>1.8378595723164685E-2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
+      <c r="A22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="B22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D22">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>1.8378595723164685E-2</v>
-      </c>
-      <c r="H22" t="str">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I22" t="str">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J22" t="str">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="6"/>
@@ -2563,43 +4001,43 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0183785957231647, _, _, _, _,</v>
+        <v xml:space="preserve">  0.008, 0.008, 0.008, 0.008, _,</v>
       </c>
       <c r="T22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>3.3914566363212231E-2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>3.3914566363212231E-2</v>
-      </c>
-      <c r="H23" t="str">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I23" t="str">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J23" t="str">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="6"/>
@@ -2607,43 +4045,43 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0339145663632122, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T23" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>1.9501047501036085E-2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>29</v>
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>1.9501047501036085E-2</v>
-      </c>
-      <c r="H24" t="str">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I24" t="str">
+        <v>0</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J24" t="str">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="6"/>
@@ -2651,24 +4089,24 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0.0195010475010361, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T24" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -2677,17 +4115,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" t="str">
+      <c r="H25">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I25" t="str">
+        <v>0</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J25" t="str">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="6"/>
@@ -2695,24 +4133,24 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T25" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -2721,17 +4159,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H26" t="str">
+      <c r="H26">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I26" t="str">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J26" t="str">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="6"/>
@@ -2739,24 +4177,24 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T26" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
@@ -2765,17 +4203,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H27" t="str">
+      <c r="H27">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I27" t="str">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J27" t="str">
+        <v>0</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="6"/>
@@ -2783,24 +4221,24 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T27" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -2809,17 +4247,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" t="str">
+      <c r="H28">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I28" t="str">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J28" t="str">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="6"/>
@@ -2827,24 +4265,24 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T28" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>29</v>
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -2853,17 +4291,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" t="str">
+      <c r="H29">
         <f t="shared" si="3"/>
-        <v>_</v>
-      </c>
-      <c r="I29" t="str">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="4"/>
-        <v>_</v>
-      </c>
-      <c r="J29" t="str">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="5"/>
-        <v>_</v>
+        <v>0</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="6"/>
@@ -2871,10 +4309,10 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  0, _, _, _, _,</v>
+        <v xml:space="preserve">  0, 0, 0, 0, _,</v>
       </c>
       <c r="T29" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2970,7 +4408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD19"/>
   <sheetViews>

</xml_diff>

<commit_message>
update biomass distribution scaling spring and fall, change movement related params
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -18,7 +18,7 @@
     <sheet name="3D_init_changer" sheetId="1" r:id="rId4"/>
     <sheet name="2D_init_changer" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -779,7 +779,7 @@
         <v>_</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M31" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
+        <f t="shared" ref="M3:M30" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
         <v xml:space="preserve">  0.299, _, _, _, _,</v>
       </c>
       <c r="T3" t="s">
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="H31:K44" si="3">IF(ISNUMBER(C31),C31*$G$1, C31)</f>
+        <f t="shared" ref="I31:K31" si="3">IF(ISNUMBER(C31),C31*$G$1, C31)</f>
         <v>0</v>
       </c>
       <c r="J31">
@@ -3164,7 +3164,7 @@
         <v>_</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M31" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
+        <f t="shared" ref="M3:M30" si="2">"  "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","</f>
         <v xml:space="preserve">  0.171, 0.171, 0.171, 0.171, _,</v>
       </c>
       <c r="T3" t="s">

</xml_diff>

<commit_message>
update scaling, calc for init, add higher mStarve and threshold for starvation to biol file
</commit_message>
<xml_diff>
--- a/R/Init_changer.xlsx
+++ b/R/Init_changer.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3D_surfOnly" sheetId="5" r:id="rId1"/>
-    <sheet name="2D calc" sheetId="3" r:id="rId2"/>
+    <sheet name="2D calc" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
     <sheet name="3D_init_changer" sheetId="1" r:id="rId4"/>
     <sheet name="2D_init_changer" sheetId="2" r:id="rId5"/>
@@ -265,7 +265,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +304,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,30 +382,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -678,13 +695,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="9.140625" style="10"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -711,7 +728,7 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="5">
         <v>0</v>
       </c>
       <c r="G2">
@@ -758,7 +775,7 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3">
@@ -802,7 +819,7 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="5">
         <v>2</v>
       </c>
       <c r="G4">
@@ -846,7 +863,7 @@
       <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
@@ -890,7 +907,7 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6">
@@ -933,7 +950,7 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="5">
         <v>5</v>
       </c>
       <c r="G7" t="s">
@@ -977,7 +994,7 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="5">
         <v>6</v>
       </c>
       <c r="G8" t="s">
@@ -1021,7 +1038,7 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="5">
         <v>7</v>
       </c>
       <c r="G9">
@@ -1065,7 +1082,7 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="5">
         <v>8</v>
       </c>
       <c r="G10" t="s">
@@ -1109,7 +1126,7 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="5">
         <v>9</v>
       </c>
       <c r="G11" t="s">
@@ -1153,7 +1170,7 @@
       <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="5">
         <v>10</v>
       </c>
       <c r="G12" t="s">
@@ -1197,7 +1214,7 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="5">
         <v>11</v>
       </c>
       <c r="G13" t="s">
@@ -1241,7 +1258,7 @@
       <c r="E14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="5">
         <v>12</v>
       </c>
       <c r="G14" t="s">
@@ -1285,7 +1302,7 @@
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="5">
         <v>13</v>
       </c>
       <c r="G15">
@@ -1329,7 +1346,7 @@
       <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="5">
         <v>14</v>
       </c>
       <c r="G16" t="s">
@@ -1373,7 +1390,7 @@
       <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="5">
         <v>15</v>
       </c>
       <c r="G17" t="s">
@@ -1417,7 +1434,7 @@
       <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="5">
         <v>16</v>
       </c>
       <c r="G18" t="s">
@@ -1461,7 +1478,7 @@
       <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="5">
         <v>17</v>
       </c>
       <c r="G19" t="s">
@@ -1505,7 +1522,7 @@
       <c r="E20" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="5">
         <v>18</v>
       </c>
       <c r="G20" t="s">
@@ -1549,7 +1566,7 @@
       <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="5">
         <v>19</v>
       </c>
       <c r="G21" t="s">
@@ -1593,7 +1610,7 @@
       <c r="E22" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="5">
         <v>20</v>
       </c>
       <c r="G22" t="s">
@@ -1637,7 +1654,7 @@
       <c r="E23" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="5">
         <v>21</v>
       </c>
       <c r="G23" t="s">
@@ -1681,7 +1698,7 @@
       <c r="E24" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="5">
         <v>22</v>
       </c>
       <c r="G24" t="s">
@@ -1725,7 +1742,7 @@
       <c r="E25" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="5">
         <v>23</v>
       </c>
       <c r="G25">
@@ -1772,7 +1789,7 @@
       <c r="E26" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="5">
         <v>24</v>
       </c>
       <c r="G26">
@@ -1819,7 +1836,7 @@
       <c r="E27" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="5">
         <v>25</v>
       </c>
       <c r="G27">
@@ -1866,7 +1883,7 @@
       <c r="E28" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="5">
         <v>26</v>
       </c>
       <c r="G28">
@@ -1913,7 +1930,7 @@
       <c r="E29" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="5">
         <v>27</v>
       </c>
       <c r="G29">
@@ -1960,7 +1977,7 @@
       <c r="E30" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="5">
         <v>28</v>
       </c>
       <c r="G30">
@@ -2007,7 +2024,7 @@
       <c r="E31" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="5">
         <v>29</v>
       </c>
       <c r="G31">
@@ -2047,765 +2064,767 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="8">
         <v>12647072876</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>12286957937</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="8">
         <v>29971254486</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="8">
         <v>13938887160</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="8">
         <v>3686010853</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="8">
         <v>11079367895</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="8">
         <v>19434502995</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="8">
         <v>10361542520</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="8">
         <v>6455559422</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="8">
         <v>17316802511</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="8">
         <v>11225017827</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="8">
         <v>15989283041</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="8">
         <v>4282287423</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="8">
         <v>14161620805</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="8">
         <v>12608709589</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="8">
         <v>9175347755</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="8">
         <v>11324453301</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="8">
         <v>5030841128</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="8">
         <v>4831356901</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="8">
         <v>17683470543</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="8">
         <v>9957085306</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="8">
         <v>6033778736</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="8">
         <v>17242902545</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="8">
         <v>173026053</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="8">
         <v>294595432</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="8">
         <v>35556339824</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="8">
         <v>17529276725</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="8">
         <v>26033456848</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="8">
         <v>40232596619</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AD2" s="8">
         <v>27427742420</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="7">
         <v>0.38900000000000001</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="7">
         <v>0.71199999999999997</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <v>0.38900000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>0.38900000000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <v>0.38900000000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <v>0.38900000000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <v>0.56200000000000006</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>0</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="9">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7">
         <v>9.4100000000000003E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>0.22950000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>0.10680000000000001</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="7">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>8.4900000000000003E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="7">
         <v>0.1489</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="7">
         <v>7.9399999999999998E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="7">
         <v>4.9399999999999999E-2</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
         <v>0.1085</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <v>7.0300000000000001E-2</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0</v>
+      </c>
+      <c r="S11" s="7">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0</v>
+      </c>
+      <c r="U11" s="7">
+        <v>0</v>
+      </c>
+      <c r="V11" s="7">
+        <v>0</v>
+      </c>
+      <c r="W11" s="7">
+        <v>0</v>
+      </c>
+      <c r="X11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="10">
         <v>1000000000000000</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="11">
         <f>$A$13*A11/20/5.7/A2</f>
         <v>0</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ref="B15:AD15" si="0">$A$13*B11/20/5.7/B2</f>
+      <c r="B15" s="11">
+        <f>$A$13*B11/20/5.7/B2</f>
         <v>67.180062040056782</v>
       </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
+      <c r="C15" s="11">
+        <f>$A$13*C11/20/5.7/C2</f>
         <v>67.16962400346695</v>
       </c>
-      <c r="D15" s="2">
-        <f t="shared" si="0"/>
+      <c r="D15" s="11">
+        <f>$A$13*D11/20/5.7/D2</f>
         <v>67.210681491961935</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" si="0"/>
+      <c r="E15" s="11">
+        <f>$A$13*E11/20/5.7/E2</f>
         <v>67.110063132695714</v>
       </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
+      <c r="F15" s="11">
+        <f>$A$13*F11/20/5.7/F2</f>
         <v>67.218351187828588</v>
       </c>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
+      <c r="G15" s="11">
+        <f>$A$13*G11/20/5.7/G2</f>
         <v>67.2072937091949</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
+      <c r="H15" s="11">
+        <f>$A$13*H11/20/5.7/H2</f>
         <v>67.218874672935797</v>
       </c>
-      <c r="I15" s="2">
-        <f t="shared" si="0"/>
+      <c r="I15" s="11">
+        <f>$A$13*I11/20/5.7/I2</f>
         <v>67.125605235166759</v>
       </c>
-      <c r="J15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="0"/>
+      <c r="J15" s="11">
+        <f>$A$13*J11/20/5.7/J2</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <f>$A$13*K11/20/5.7/K2</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <f>$A$13*L11/20/5.7/L2</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="11">
+        <f>$A$13*M11/20/5.7/M2</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="11">
+        <f>$A$13*N11/20/5.7/N2</f>
         <v>67.206600082730588</v>
       </c>
-      <c r="O15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
-        <f t="shared" si="0"/>
+      <c r="O15" s="11">
+        <f>$A$13*O11/20/5.7/O2</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="11">
+        <f>$A$13*P11/20/5.7/P2</f>
         <v>67.209078405842575</v>
       </c>
-      <c r="Q15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="2">
+      <c r="Q15" s="11">
+        <f>$A$13*Q11/20/5.7/Q2</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="11">
         <f>$A$13*R11/20/5.7/R2</f>
         <v>0</v>
       </c>
-      <c r="S15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="S15" s="11">
+        <f>$A$13*S11/20/5.7/S2</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="11">
+        <f>$A$13*T11/20/5.7/T2</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="11">
+        <f>$A$13*U11/20/5.7/U2</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="11">
+        <f>$A$13*V11/20/5.7/V2</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="11">
+        <f>$A$13*W11/20/5.7/W2</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="11">
+        <f>$A$13*X11/20/5.7/X2</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="11">
+        <f>$A$13*Y11/20/5.7/Y2</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="11">
+        <f>$A$13*Z11/20/5.7/Z2</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="11">
+        <f>$A$13*AA11/20/5.7/AA2</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="11">
+        <f>$A$13*AB11/20/5.7/AB2</f>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="11">
+        <f>$A$13*AC11/20/5.7/AC2</f>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="11">
+        <f>$A$13*AD11/20/5.7/AD2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
         <f>IF(ISNUMBER(A15),A15,_)</f>
         <v>0</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="12">
         <f>IF(ISNUMBER(B15),B15,_)</f>
         <v>67.180062040056782</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="12">
         <f>IF(ISNUMBER(C15),C15,_)</f>
         <v>67.16962400346695</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="12">
         <f>IF(ISNUMBER(D15),D15,_)</f>
         <v>67.210681491961935</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="12">
         <f>IF(ISNUMBER(E15),E15,_)</f>
         <v>67.110063132695714</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="12">
         <f>IF(ISNUMBER(F15),F15,_)</f>
         <v>67.218351187828588</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="12">
         <f>IF(ISNUMBER(G15),G15,_)</f>
         <v>67.2072937091949</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="12">
         <f>IF(ISNUMBER(H15),H15,_)</f>
         <v>67.218874672935797</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="12">
         <f>IF(ISNUMBER(I15),I15,_)</f>
         <v>67.125605235166759</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="12">
         <f>IF(ISNUMBER(J15),J15,_)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="12">
         <f>IF(ISNUMBER(K15),K15,_)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="12">
         <f>IF(ISNUMBER(L15),L15,_)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="12">
         <f>IF(ISNUMBER(M15),M15,_)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="12">
         <f>IF(ISNUMBER(N15),N15,_)</f>
         <v>67.206600082730588</v>
       </c>
-      <c r="O16" s="8">
+      <c r="O16" s="12">
         <f>IF(ISNUMBER(O15),O15,_)</f>
         <v>0</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="12">
         <f>IF(ISNUMBER(P15),P15,_)</f>
         <v>67.209078405842575</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="Q16" s="12">
         <f>IF(ISNUMBER(Q15),Q15,_)</f>
         <v>0</v>
       </c>
-      <c r="R16" s="8">
+      <c r="R16" s="12">
         <f>IF(ISNUMBER(R15),R15,_)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="8">
+      <c r="S16" s="12">
         <f>IF(ISNUMBER(S15),S15,_)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="8">
+      <c r="T16" s="12">
         <f>IF(ISNUMBER(T15),T15,_)</f>
         <v>0</v>
       </c>
-      <c r="U16" s="8">
+      <c r="U16" s="12">
         <f>IF(ISNUMBER(U15),U15,_)</f>
         <v>0</v>
       </c>
-      <c r="V16" s="8">
+      <c r="V16" s="12">
         <f>IF(ISNUMBER(V15),V15,_)</f>
         <v>0</v>
       </c>
-      <c r="W16" s="8">
+      <c r="W16" s="12">
         <f>IF(ISNUMBER(W15),W15,_)</f>
         <v>0</v>
       </c>
-      <c r="X16" s="8">
+      <c r="X16" s="12">
         <f>IF(ISNUMBER(X15),X15,_)</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="8">
+      <c r="Y16" s="12">
         <f>IF(ISNUMBER(Y15),Y15,_)</f>
         <v>0</v>
       </c>
-      <c r="Z16" s="8">
+      <c r="Z16" s="12">
         <f>IF(ISNUMBER(Z15),Z15,_)</f>
         <v>0</v>
       </c>
-      <c r="AA16" s="8">
+      <c r="AA16" s="12">
         <f>IF(ISNUMBER(AA15),AA15,_)</f>
         <v>0</v>
       </c>
-      <c r="AB16" s="8">
+      <c r="AB16" s="12">
         <f>IF(ISNUMBER(AB15),AB15,_)</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="8">
+      <c r="AC16" s="12">
         <f>IF(ISNUMBER(AC15),AC15,_)</f>
         <v>0</v>
       </c>
-      <c r="AD16" s="8">
+      <c r="AD16" s="12">
         <f>IF(ISNUMBER(AD15),AD15,_)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
+      <c r="A18" s="7" t="str">
         <f>"  "&amp;A16&amp;", "&amp;B16&amp;", "&amp;C16&amp;", "&amp;D16&amp;", "&amp;E16&amp;", "&amp;F16&amp;", "&amp;G16&amp;", "&amp;H16&amp;", "&amp;I16&amp;", "&amp;J16&amp;", "&amp;K16&amp;", "&amp;L16&amp;", "&amp;M16&amp;", "&amp;N16&amp;", "&amp;O16&amp;", "&amp;P16&amp;", "&amp;Q16&amp;", "&amp;R16&amp;", "&amp;S16&amp;", "&amp;T16&amp;", "&amp;U16&amp;", "&amp;V16&amp;", "&amp;W16&amp;", "&amp;X16&amp;", "&amp;Y16&amp;", "&amp;Z16&amp;", "&amp;AA16&amp;", "&amp;AB16&amp;", "&amp;AC16&amp;", "&amp;AD16&amp;" ;"</f>
         <v xml:space="preserve">  0, 67.1800620400568, 67.169624003467, 67.2106814919619, 67.1100631326957, 67.2183511878286, 67.2072937091949, 67.2188746729358, 67.1256052351668, 0, 0, 0, 0, 67.2066000827306, 0, 67.2090784058426, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ;</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>0</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="9">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7">
         <v>3.8412785569043447E-5</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>1.8367546472103407E-2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>0.13049277850702132</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="7">
         <v>4.7251947196421864E-3</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="7">
         <v>7.6064601398792629E-4</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="7">
         <v>1.8486370070418463E-3</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="7">
         <v>3.9807699200918329E-3</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="7">
         <v>0.18259307925860729</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="7">
         <v>6.4567875126470345E-3</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="7">
         <v>4.5143082014423895E-3</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="7">
         <v>0.10275523558662426</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="7">
         <v>1.4705889237647663E-4</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="7">
         <v>5.3006863024427968E-2</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="7">
         <v>1.4183515334295856E-2</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="7">
         <v>1.7270388414270525E-2</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="7">
         <v>6.169684274222164E-3</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="7">
         <v>1.6281006727388105E-2</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="7">
         <v>1.6281006727388105E-2</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="7">
         <v>4.3750896401474199E-2</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="7">
         <v>5.4311918102124913E-2</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="7">
         <v>0.19490523910211674</v>
       </c>
-      <c r="W22">
+      <c r="W22" s="7">
         <v>0.23321205139330659</v>
       </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <v>0</v>
-      </c>
-      <c r="AB22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <v>0</v>
-      </c>
-      <c r="AD22">
+      <c r="X22" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+      <c r="A24" s="7" t="str">
         <f>"  "&amp;A22&amp;", "&amp;B22&amp;", "&amp;C22&amp;", "&amp;D22&amp;", "&amp;E22&amp;", "&amp;F22&amp;", "&amp;G22&amp;", "&amp;H22&amp;", "&amp;I22&amp;", "&amp;J22&amp;", "&amp;K22&amp;", "&amp;L22&amp;", "&amp;M22&amp;", "&amp;N22&amp;", "&amp;O22&amp;", "&amp;P22&amp;", "&amp;Q22&amp;", "&amp;R22&amp;", "&amp;S22&amp;", "&amp;T22&amp;", "&amp;U22&amp;", "&amp;V22&amp;", "&amp;W22&amp;", "&amp;X22&amp;", "&amp;Y22&amp;", "&amp;Z22&amp;", "&amp;AA22&amp;", "&amp;AB22&amp;", "&amp;AC22&amp;", "&amp;AD22&amp;" ;"</f>
         <v xml:space="preserve">  0, 3.84127855690434E-05, 0.0183675464721034, 0.130492778507021, 0.00472519471964219, 0.000760646013987926, 0.00184863700704185, 0.00398076992009183, 0.182593079258607, 0.00645678751264703, 0.00451430820144239, 0.102755235586624, 0.000147058892376477, 0.053006863024428, 0.0141835153342959, 0.0172703884142705, 0.00616968427422216, 0.0162810067273881, 0.0162810067273881, 0.0437508964014742, 0.0543119181021249, 0.194905239102117, 0.233212051393307, 0, 0, 0, 0, 0, 0, 0 ;</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="10">
         <v>1000000000000000</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="11">
         <v>4000000000000000</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="11">
         <v>63000000000000</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2826,7 +2845,7 @@
   <sheetData>
     <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3">
@@ -2924,7 +2943,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4">
@@ -4316,7 +4335,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="4">
         <v>0</v>
       </c>
       <c r="B30" t="s">
@@ -4360,7 +4379,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="4">
         <v>0</v>
       </c>
       <c r="B31" t="s">
@@ -4419,94 +4438,94 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
+      <c r="A1" s="2">
         <v>12647072876</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>12286957937</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>29971254486</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>13938887160</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>3686010853</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>11079367895</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>19434502995</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>10361542520</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>6455559422</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>17316802511</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>11225017827</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>15989283041</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>4282287423</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="2">
         <v>14161620805</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="2">
         <v>12608709589</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="2">
         <v>9175347755</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q1" s="2">
         <v>11324453301</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R1" s="2">
         <v>5030841128</v>
       </c>
-      <c r="S1" s="3">
+      <c r="S1" s="2">
         <v>4831356901</v>
       </c>
-      <c r="T1" s="3">
+      <c r="T1" s="2">
         <v>17683470543</v>
       </c>
-      <c r="U1" s="3">
+      <c r="U1" s="2">
         <v>9957085306</v>
       </c>
-      <c r="V1" s="3">
+      <c r="V1" s="2">
         <v>6033778736</v>
       </c>
-      <c r="W1" s="3">
+      <c r="W1" s="2">
         <v>17242902545</v>
       </c>
-      <c r="X1" s="3">
+      <c r="X1" s="2">
         <v>173026053</v>
       </c>
-      <c r="Y1" s="3">
+      <c r="Y1" s="2">
         <v>294595432</v>
       </c>
-      <c r="Z1" s="3">
+      <c r="Z1" s="2">
         <v>35556339824</v>
       </c>
-      <c r="AA1" s="3">
+      <c r="AA1" s="2">
         <v>17529276725</v>
       </c>
-      <c r="AB1" s="3">
+      <c r="AB1" s="2">
         <v>26033456848</v>
       </c>
-      <c r="AC1" s="3">
+      <c r="AC1" s="2">
         <v>40232596619</v>
       </c>
-      <c r="AD1" s="3">
+      <c r="AD1" s="2">
         <v>27427742420</v>
       </c>
     </row>

</xml_diff>